<commit_message>
Add source data for Supplementary Fig S2
</commit_message>
<xml_diff>
--- a/Source_Data/Fig_S2.xlsx
+++ b/Source_Data/Fig_S2.xlsx
@@ -1514,10 +1514,10 @@
         <v>5</v>
       </c>
       <c r="B2" t="n">
-        <v>25.7490260597225</v>
+        <v>-38.192462664229</v>
       </c>
       <c r="C2" t="n">
-        <v>-22.7890857369864</v>
+        <v>-31.9969100711597</v>
       </c>
       <c r="D2" t="s">
         <v>6</v>
@@ -1531,10 +1531,10 @@
         <v>8</v>
       </c>
       <c r="B3" t="n">
-        <v>5.26128002381634</v>
+        <v>57.352288024364</v>
       </c>
       <c r="C3" t="n">
-        <v>2.96904785161543</v>
+        <v>-12.1673011850424</v>
       </c>
       <c r="D3" t="s">
         <v>9</v>
@@ -1548,10 +1548,10 @@
         <v>10</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.25466676720031</v>
+        <v>52.801326523277</v>
       </c>
       <c r="C4" t="n">
-        <v>26.6437180704065</v>
+        <v>-8.71462178302717</v>
       </c>
       <c r="D4" t="s">
         <v>9</v>
@@ -1565,10 +1565,10 @@
         <v>11</v>
       </c>
       <c r="B5" t="n">
-        <v>33.9608057546067</v>
+        <v>49.9320312241605</v>
       </c>
       <c r="C5" t="n">
-        <v>-6.98824571411541</v>
+        <v>6.9793042511732</v>
       </c>
       <c r="D5" t="s">
         <v>9</v>
@@ -1582,10 +1582,10 @@
         <v>12</v>
       </c>
       <c r="B6" t="n">
-        <v>35.2401616075227</v>
+        <v>44.8075216143318</v>
       </c>
       <c r="C6" t="n">
-        <v>21.4693371672315</v>
+        <v>35.0265080214091</v>
       </c>
       <c r="D6" t="s">
         <v>9</v>
@@ -1599,10 +1599,10 @@
         <v>13</v>
       </c>
       <c r="B7" t="n">
-        <v>-30.9582493514868</v>
+        <v>61.5280370106319</v>
       </c>
       <c r="C7" t="n">
-        <v>0.262600024090476</v>
+        <v>-11.9622601657963</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
@@ -1616,10 +1616,10 @@
         <v>15</v>
       </c>
       <c r="B8" t="n">
-        <v>-4.00005146270183</v>
+        <v>73.123524054261</v>
       </c>
       <c r="C8" t="n">
-        <v>-15.4195086254178</v>
+        <v>-27.651945820609</v>
       </c>
       <c r="D8" t="s">
         <v>9</v>
@@ -1633,10 +1633,10 @@
         <v>16</v>
       </c>
       <c r="B9" t="n">
-        <v>-15.9564597138717</v>
+        <v>65.9472693633932</v>
       </c>
       <c r="C9" t="n">
-        <v>-10.3963289325659</v>
+        <v>-21.9579342101448</v>
       </c>
       <c r="D9" t="s">
         <v>9</v>
@@ -1650,10 +1650,10 @@
         <v>17</v>
       </c>
       <c r="B10" t="n">
-        <v>12.9135462804211</v>
+        <v>-82.3032050632391</v>
       </c>
       <c r="C10" t="n">
-        <v>-11.2422822828472</v>
+        <v>14.153816025237</v>
       </c>
       <c r="D10" t="s">
         <v>6</v>
@@ -1667,10 +1667,10 @@
         <v>18</v>
       </c>
       <c r="B11" t="n">
-        <v>-10.2502564138699</v>
+        <v>-14.0466932284881</v>
       </c>
       <c r="C11" t="n">
-        <v>8.88205500542942</v>
+        <v>-33.9895202275196</v>
       </c>
       <c r="D11" t="s">
         <v>6</v>
@@ -1684,10 +1684,10 @@
         <v>19</v>
       </c>
       <c r="B12" t="n">
-        <v>-13.3535755494055</v>
+        <v>-40.7075247371302</v>
       </c>
       <c r="C12" t="n">
-        <v>-6.36793417786376</v>
+        <v>-18.8781591063855</v>
       </c>
       <c r="D12" t="s">
         <v>6</v>
@@ -1701,10 +1701,10 @@
         <v>20</v>
       </c>
       <c r="B13" t="n">
-        <v>-5.50222850408824</v>
+        <v>43.6663630591544</v>
       </c>
       <c r="C13" t="n">
-        <v>-16.2397242576215</v>
+        <v>10.4063455737228</v>
       </c>
       <c r="D13" t="s">
         <v>9</v>
@@ -1718,10 +1718,10 @@
         <v>21</v>
       </c>
       <c r="B14" t="n">
-        <v>13.3380137766398</v>
+        <v>-76.8303706960225</v>
       </c>
       <c r="C14" t="n">
-        <v>16.6601385039702</v>
+        <v>20.8495590463887</v>
       </c>
       <c r="D14" t="s">
         <v>9</v>
@@ -1735,10 +1735,10 @@
         <v>22</v>
       </c>
       <c r="B15" t="n">
-        <v>-41.2207141521848</v>
+        <v>43.11458577159</v>
       </c>
       <c r="C15" t="n">
-        <v>15.1308257435431</v>
+        <v>50.215844449083</v>
       </c>
       <c r="D15" t="s">
         <v>9</v>
@@ -1752,10 +1752,10 @@
         <v>23</v>
       </c>
       <c r="B16" t="n">
-        <v>-4.63428361736823</v>
+        <v>53.944720807319</v>
       </c>
       <c r="C16" t="n">
-        <v>2.85284387669289</v>
+        <v>-6.78166583734848</v>
       </c>
       <c r="D16" t="s">
         <v>9</v>
@@ -1769,10 +1769,10 @@
         <v>24</v>
       </c>
       <c r="B17" t="n">
-        <v>-13.0927298868852</v>
+        <v>-40.2474322277811</v>
       </c>
       <c r="C17" t="n">
-        <v>12.924638165519</v>
+        <v>15.6233491213452</v>
       </c>
       <c r="D17" t="s">
         <v>6</v>
@@ -1786,10 +1786,10 @@
         <v>25</v>
       </c>
       <c r="B18" t="n">
-        <v>-12.6333957874623</v>
+        <v>53.4910491027984</v>
       </c>
       <c r="C18" t="n">
-        <v>-4.77235995258644</v>
+        <v>1.3841917868491</v>
       </c>
       <c r="D18" t="s">
         <v>9</v>
@@ -1803,10 +1803,10 @@
         <v>26</v>
       </c>
       <c r="B19" t="n">
-        <v>0.441570950081597</v>
+        <v>50.6920050112546</v>
       </c>
       <c r="C19" t="n">
-        <v>-17.9326337397736</v>
+        <v>7.68838997544001</v>
       </c>
       <c r="D19" t="s">
         <v>9</v>
@@ -1820,10 +1820,10 @@
         <v>27</v>
       </c>
       <c r="B20" t="n">
-        <v>-7.64110279444547</v>
+        <v>-17.9422319801293</v>
       </c>
       <c r="C20" t="n">
-        <v>12.489944651804</v>
+        <v>-20.5492457305544</v>
       </c>
       <c r="D20" t="s">
         <v>6</v>
@@ -1837,10 +1837,10 @@
         <v>28</v>
       </c>
       <c r="B21" t="n">
-        <v>-4.58766024523132</v>
+        <v>25.5661774308537</v>
       </c>
       <c r="C21" t="n">
-        <v>-4.12957372574951</v>
+        <v>59.0450690031914</v>
       </c>
       <c r="D21" t="s">
         <v>9</v>
@@ -1854,10 +1854,10 @@
         <v>29</v>
       </c>
       <c r="B22" t="n">
-        <v>-8.86892156291011</v>
+        <v>39.2311679673443</v>
       </c>
       <c r="C22" t="n">
-        <v>3.3821661991513</v>
+        <v>-14.1006297566886</v>
       </c>
       <c r="D22" t="s">
         <v>9</v>
@@ -1871,10 +1871,10 @@
         <v>30</v>
       </c>
       <c r="B23" t="n">
-        <v>-9.06363274625637</v>
+        <v>-5.85431977748975</v>
       </c>
       <c r="C23" t="n">
-        <v>7.40386782663078</v>
+        <v>-23.5377250184842</v>
       </c>
       <c r="D23" t="s">
         <v>6</v>
@@ -1888,10 +1888,10 @@
         <v>31</v>
       </c>
       <c r="B24" t="n">
-        <v>-17.1763043009118</v>
+        <v>55.4298693239783</v>
       </c>
       <c r="C24" t="n">
-        <v>6.52982813471607</v>
+        <v>3.7276053777404</v>
       </c>
       <c r="D24" t="s">
         <v>6</v>
@@ -1905,10 +1905,10 @@
         <v>32</v>
       </c>
       <c r="B25" t="n">
-        <v>3.04554879560479</v>
+        <v>42.721498879686</v>
       </c>
       <c r="C25" t="n">
-        <v>-16.2793849829207</v>
+        <v>42.3256809157712</v>
       </c>
       <c r="D25" t="s">
         <v>9</v>
@@ -1922,10 +1922,10 @@
         <v>33</v>
       </c>
       <c r="B26" t="n">
-        <v>-10.2124373589642</v>
+        <v>-26.742062959843</v>
       </c>
       <c r="C26" t="n">
-        <v>-10.1270012911077</v>
+        <v>-3.00912654141937</v>
       </c>
       <c r="D26" t="s">
         <v>6</v>
@@ -1939,10 +1939,10 @@
         <v>34</v>
       </c>
       <c r="B27" t="n">
-        <v>17.7747159150966</v>
+        <v>53.0984404870611</v>
       </c>
       <c r="C27" t="n">
-        <v>37.9629172378667</v>
+        <v>-14.7067117754942</v>
       </c>
       <c r="D27" t="s">
         <v>9</v>
@@ -1956,10 +1956,10 @@
         <v>35</v>
       </c>
       <c r="B28" t="n">
-        <v>-2.62761085660758</v>
+        <v>-26.4902962170545</v>
       </c>
       <c r="C28" t="n">
-        <v>-0.732256092901718</v>
+        <v>14.8530839309816</v>
       </c>
       <c r="D28" t="s">
         <v>6</v>
@@ -1973,10 +1973,10 @@
         <v>36</v>
       </c>
       <c r="B29" t="n">
-        <v>-11.1759829015368</v>
+        <v>-57.2206814662163</v>
       </c>
       <c r="C29" t="n">
-        <v>-8.70002255020288</v>
+        <v>37.1018276300059</v>
       </c>
       <c r="D29" t="s">
         <v>6</v>
@@ -1990,10 +1990,10 @@
         <v>37</v>
       </c>
       <c r="B30" t="n">
-        <v>21.8470751132213</v>
+        <v>28.9001139652814</v>
       </c>
       <c r="C30" t="n">
-        <v>24.7260608946821</v>
+        <v>56.0610733697647</v>
       </c>
       <c r="D30" t="s">
         <v>6</v>
@@ -2007,10 +2007,10 @@
         <v>38</v>
       </c>
       <c r="B31" t="n">
-        <v>-11.1299411361858</v>
+        <v>-36.0767391380428</v>
       </c>
       <c r="C31" t="n">
-        <v>-1.43402754839762</v>
+        <v>0.767236339000703</v>
       </c>
       <c r="D31" t="s">
         <v>6</v>
@@ -2024,10 +2024,10 @@
         <v>39</v>
       </c>
       <c r="B32" t="n">
-        <v>18.5677246860928</v>
+        <v>53.737475624114</v>
       </c>
       <c r="C32" t="n">
-        <v>1.84262254683242</v>
+        <v>0.927475352677161</v>
       </c>
       <c r="D32" t="s">
         <v>9</v>
@@ -2041,10 +2041,10 @@
         <v>40</v>
       </c>
       <c r="B33" t="n">
-        <v>-16.3565273060052</v>
+        <v>-43.1536229482775</v>
       </c>
       <c r="C33" t="n">
-        <v>-0.402931717134896</v>
+        <v>-17.001720042389</v>
       </c>
       <c r="D33" t="s">
         <v>6</v>
@@ -2058,10 +2058,10 @@
         <v>41</v>
       </c>
       <c r="B34" t="n">
-        <v>10.0039146840886</v>
+        <v>-45.2481528905231</v>
       </c>
       <c r="C34" t="n">
-        <v>-2.67784102785543</v>
+        <v>3.01453686046592</v>
       </c>
       <c r="D34" t="s">
         <v>6</v>
@@ -2075,10 +2075,10 @@
         <v>42</v>
       </c>
       <c r="B35" t="n">
-        <v>16.7332276599321</v>
+        <v>-53.775025585855</v>
       </c>
       <c r="C35" t="n">
-        <v>-10.0563543408448</v>
+        <v>-11.8189781039757</v>
       </c>
       <c r="D35" t="s">
         <v>6</v>
@@ -2092,10 +2092,10 @@
         <v>43</v>
       </c>
       <c r="B36" t="n">
-        <v>11.1596075878163</v>
+        <v>-41.03357911588</v>
       </c>
       <c r="C36" t="n">
-        <v>32.3746550216202</v>
+        <v>-9.43307132566459</v>
       </c>
       <c r="D36" t="s">
         <v>6</v>
@@ -2109,10 +2109,10 @@
         <v>44</v>
       </c>
       <c r="B37" t="n">
-        <v>8.9439058010641</v>
+        <v>-74.1610421583284</v>
       </c>
       <c r="C37" t="n">
-        <v>-13.3150910157408</v>
+        <v>8.80674742305451</v>
       </c>
       <c r="D37" t="s">
         <v>6</v>
@@ -2126,10 +2126,10 @@
         <v>45</v>
       </c>
       <c r="B38" t="n">
-        <v>-0.498080136348114</v>
+        <v>-57.8339791745899</v>
       </c>
       <c r="C38" t="n">
-        <v>-4.39105672392249</v>
+        <v>-10.8742622360481</v>
       </c>
       <c r="D38" t="s">
         <v>6</v>
@@ -2143,10 +2143,10 @@
         <v>46</v>
       </c>
       <c r="B39" t="n">
-        <v>-5.41509709754544</v>
+        <v>58.9576618517587</v>
       </c>
       <c r="C39" t="n">
-        <v>-13.900786807896</v>
+        <v>-18.9382124195365</v>
       </c>
       <c r="D39" t="s">
         <v>9</v>
@@ -2160,10 +2160,10 @@
         <v>47</v>
       </c>
       <c r="B40" t="n">
-        <v>5.7583694984118</v>
+        <v>-63.2751057940912</v>
       </c>
       <c r="C40" t="n">
-        <v>4.42432924988639</v>
+        <v>9.77694348029231</v>
       </c>
       <c r="D40" t="s">
         <v>6</v>
@@ -2177,10 +2177,10 @@
         <v>48</v>
       </c>
       <c r="B41" t="n">
-        <v>-5.77834448421839</v>
+        <v>-11.107860300321</v>
       </c>
       <c r="C41" t="n">
-        <v>0.916294543765368</v>
+        <v>11.1713396689842</v>
       </c>
       <c r="D41" t="s">
         <v>6</v>
@@ -2194,10 +2194,10 @@
         <v>49</v>
       </c>
       <c r="B42" t="n">
-        <v>9.85433260721774</v>
+        <v>-54.0928729507576</v>
       </c>
       <c r="C42" t="n">
-        <v>-1.75387332448797</v>
+        <v>-16.4626892534548</v>
       </c>
       <c r="D42" t="s">
         <v>6</v>
@@ -2211,10 +2211,10 @@
         <v>50</v>
       </c>
       <c r="B43" t="n">
-        <v>3.02687274129258</v>
+        <v>-41.8874232527873</v>
       </c>
       <c r="C43" t="n">
-        <v>-12.7378786939424</v>
+        <v>-52.4584539285249</v>
       </c>
       <c r="D43" t="s">
         <v>6</v>
@@ -2228,10 +2228,10 @@
         <v>51</v>
       </c>
       <c r="B44" t="n">
-        <v>-4.48535578911945</v>
+        <v>52.9214797796489</v>
       </c>
       <c r="C44" t="n">
-        <v>-3.57183466067758</v>
+        <v>23.6255752612424</v>
       </c>
       <c r="D44" t="s">
         <v>9</v>
@@ -2245,10 +2245,10 @@
         <v>52</v>
       </c>
       <c r="B45" t="n">
-        <v>52.0316852179225</v>
+        <v>18.9724340165093</v>
       </c>
       <c r="C45" t="n">
-        <v>-9.45297486788903</v>
+        <v>57.1619944912683</v>
       </c>
       <c r="D45" t="s">
         <v>6</v>
@@ -2262,10 +2262,10 @@
         <v>53</v>
       </c>
       <c r="B46" t="n">
-        <v>-16.4013917865431</v>
+        <v>62.9550683953301</v>
       </c>
       <c r="C46" t="n">
-        <v>6.22472223374204</v>
+        <v>-7.90477104629685</v>
       </c>
       <c r="D46" t="s">
         <v>9</v>
@@ -2279,10 +2279,10 @@
         <v>54</v>
       </c>
       <c r="B47" t="n">
-        <v>25.4821405295556</v>
+        <v>54.4799865097361</v>
       </c>
       <c r="C47" t="n">
-        <v>27.5641575345579</v>
+        <v>-11.9583450433625</v>
       </c>
       <c r="D47" t="s">
         <v>9</v>
@@ -2296,10 +2296,10 @@
         <v>55</v>
       </c>
       <c r="B48" t="n">
-        <v>2.47672234958596</v>
+        <v>-17.9461179629582</v>
       </c>
       <c r="C48" t="n">
-        <v>-18.6719209089467</v>
+        <v>28.6919588299204</v>
       </c>
       <c r="D48" t="s">
         <v>6</v>
@@ -2313,10 +2313,10 @@
         <v>56</v>
       </c>
       <c r="B49" t="n">
-        <v>6.0344204682706</v>
+        <v>-5.92478793843251</v>
       </c>
       <c r="C49" t="n">
-        <v>14.78456063703</v>
+        <v>-8.94890220923819</v>
       </c>
       <c r="D49" t="s">
         <v>6</v>
@@ -2330,10 +2330,10 @@
         <v>57</v>
       </c>
       <c r="B50" t="n">
-        <v>-30.4264175034651</v>
+        <v>67.3726884238663</v>
       </c>
       <c r="C50" t="n">
-        <v>17.960612088426</v>
+        <v>-20.0421947864912</v>
       </c>
       <c r="D50" t="s">
         <v>9</v>
@@ -2347,10 +2347,10 @@
         <v>58</v>
       </c>
       <c r="B51" t="n">
-        <v>-26.9353273481506</v>
+        <v>50.6277000333769</v>
       </c>
       <c r="C51" t="n">
-        <v>8.87193151939525</v>
+        <v>10.1843127403807</v>
       </c>
       <c r="D51" t="s">
         <v>9</v>
@@ -2364,10 +2364,10 @@
         <v>59</v>
       </c>
       <c r="B52" t="n">
-        <v>0.565138826412215</v>
+        <v>68.6512402368174</v>
       </c>
       <c r="C52" t="n">
-        <v>-8.30781280197506</v>
+        <v>-26.694465831123</v>
       </c>
       <c r="D52" t="s">
         <v>9</v>
@@ -2381,10 +2381,10 @@
         <v>60</v>
       </c>
       <c r="B53" t="n">
-        <v>-5.19426153656374</v>
+        <v>38.0192600071357</v>
       </c>
       <c r="C53" t="n">
-        <v>-7.31118724799215</v>
+        <v>60.3930256656626</v>
       </c>
       <c r="D53" t="s">
         <v>9</v>
@@ -2398,10 +2398,10 @@
         <v>61</v>
       </c>
       <c r="B54" t="n">
-        <v>-2.07694941998539</v>
+        <v>66.168529473779</v>
       </c>
       <c r="C54" t="n">
-        <v>4.34300459204001</v>
+        <v>-7.88204951200707</v>
       </c>
       <c r="D54" t="s">
         <v>9</v>
@@ -2415,10 +2415,10 @@
         <v>62</v>
       </c>
       <c r="B55" t="n">
-        <v>-16.802241410591</v>
+        <v>43.0022988974642</v>
       </c>
       <c r="C55" t="n">
-        <v>9.37500492903198</v>
+        <v>33.9329216110609</v>
       </c>
       <c r="D55" t="s">
         <v>9</v>
@@ -2432,10 +2432,10 @@
         <v>63</v>
       </c>
       <c r="B56" t="n">
-        <v>5.47367115017628</v>
+        <v>49.5442995312561</v>
       </c>
       <c r="C56" t="n">
-        <v>15.0368629446245</v>
+        <v>19.0348055514428</v>
       </c>
       <c r="D56" t="s">
         <v>9</v>
@@ -2449,10 +2449,10 @@
         <v>64</v>
       </c>
       <c r="B57" t="n">
-        <v>17.9905590744502</v>
+        <v>69.8223490576029</v>
       </c>
       <c r="C57" t="n">
-        <v>-2.04758651742511</v>
+        <v>-25.8658450501211</v>
       </c>
       <c r="D57" t="s">
         <v>9</v>
@@ -2466,10 +2466,10 @@
         <v>65</v>
       </c>
       <c r="B58" t="n">
-        <v>39.1137844366948</v>
+        <v>58.1505168781861</v>
       </c>
       <c r="C58" t="n">
-        <v>18.9870679716477</v>
+        <v>-19.7030113632817</v>
       </c>
       <c r="D58" t="s">
         <v>9</v>
@@ -2483,10 +2483,10 @@
         <v>66</v>
       </c>
       <c r="B59" t="n">
-        <v>17.1847528026713</v>
+        <v>48.8301287351971</v>
       </c>
       <c r="C59" t="n">
-        <v>29.3004667037397</v>
+        <v>-9.85950507443847</v>
       </c>
       <c r="D59" t="s">
         <v>9</v>
@@ -2500,10 +2500,10 @@
         <v>67</v>
       </c>
       <c r="B60" t="n">
-        <v>14.6717784298421</v>
+        <v>45.1141345173601</v>
       </c>
       <c r="C60" t="n">
-        <v>-2.14986405288824</v>
+        <v>22.3860129224683</v>
       </c>
       <c r="D60" t="s">
         <v>9</v>
@@ -2517,10 +2517,10 @@
         <v>68</v>
       </c>
       <c r="B61" t="n">
-        <v>-3.82416912615384</v>
+        <v>39.7327393087776</v>
       </c>
       <c r="C61" t="n">
-        <v>-14.5549577559492</v>
+        <v>32.8551095935992</v>
       </c>
       <c r="D61" t="s">
         <v>9</v>
@@ -2534,10 +2534,10 @@
         <v>69</v>
       </c>
       <c r="B62" t="n">
-        <v>-9.23973100494823</v>
+        <v>77.2777582678524</v>
       </c>
       <c r="C62" t="n">
-        <v>5.22071609684101</v>
+        <v>-45.8783456245864</v>
       </c>
       <c r="D62" t="s">
         <v>9</v>
@@ -2551,10 +2551,10 @@
         <v>70</v>
       </c>
       <c r="B63" t="n">
-        <v>-10.8465023597666</v>
+        <v>57.950631076557</v>
       </c>
       <c r="C63" t="n">
-        <v>-1.46503629890267</v>
+        <v>7.61912198246399</v>
       </c>
       <c r="D63" t="s">
         <v>9</v>
@@ -2568,10 +2568,10 @@
         <v>71</v>
       </c>
       <c r="B64" t="n">
-        <v>-16.1183552692176</v>
+        <v>-44.1746136355742</v>
       </c>
       <c r="C64" t="n">
-        <v>-0.960682703955081</v>
+        <v>28.2394649511763</v>
       </c>
       <c r="D64" t="s">
         <v>6</v>
@@ -2585,10 +2585,10 @@
         <v>72</v>
       </c>
       <c r="B65" t="n">
-        <v>-22.7470885211954</v>
+        <v>-22.9155720118547</v>
       </c>
       <c r="C65" t="n">
-        <v>2.60278628145739</v>
+        <v>1.70623296699086</v>
       </c>
       <c r="D65" t="s">
         <v>6</v>
@@ -2602,10 +2602,10 @@
         <v>73</v>
       </c>
       <c r="B66" t="n">
-        <v>31.4968343209992</v>
+        <v>40.4491396394997</v>
       </c>
       <c r="C66" t="n">
-        <v>8.09793815357929</v>
+        <v>39.7172674736966</v>
       </c>
       <c r="D66" t="s">
         <v>9</v>
@@ -2619,10 +2619,10 @@
         <v>74</v>
       </c>
       <c r="B67" t="n">
-        <v>8.28768613237505</v>
+        <v>-18.9963977625888</v>
       </c>
       <c r="C67" t="n">
-        <v>-22.0837795684812</v>
+        <v>10.1314841338944</v>
       </c>
       <c r="D67" t="s">
         <v>6</v>
@@ -2636,10 +2636,10 @@
         <v>75</v>
       </c>
       <c r="B68" t="n">
-        <v>25.3350219617979</v>
+        <v>28.0926554373973</v>
       </c>
       <c r="C68" t="n">
-        <v>30.2943668017421</v>
+        <v>40.7852234540245</v>
       </c>
       <c r="D68" t="s">
         <v>6</v>
@@ -2653,10 +2653,10 @@
         <v>76</v>
       </c>
       <c r="B69" t="n">
-        <v>16.3831986577588</v>
+        <v>59.5339297578381</v>
       </c>
       <c r="C69" t="n">
-        <v>3.25238187026388</v>
+        <v>-15.4589121649365</v>
       </c>
       <c r="D69" t="s">
         <v>9</v>
@@ -2670,10 +2670,10 @@
         <v>77</v>
       </c>
       <c r="B70" t="n">
-        <v>-27.2013455402437</v>
+        <v>57.608895289765</v>
       </c>
       <c r="C70" t="n">
-        <v>-15.0036484756337</v>
+        <v>-12.291271327243</v>
       </c>
       <c r="D70" t="s">
         <v>9</v>
@@ -2687,10 +2687,10 @@
         <v>78</v>
       </c>
       <c r="B71" t="n">
-        <v>-16.0573068559465</v>
+        <v>1.50254473614265</v>
       </c>
       <c r="C71" t="n">
-        <v>-17.4026895983517</v>
+        <v>37.8366297635877</v>
       </c>
       <c r="D71" t="s">
         <v>6</v>
@@ -2704,10 +2704,10 @@
         <v>79</v>
       </c>
       <c r="B72" t="n">
-        <v>11.9783385793924</v>
+        <v>63.6772293437212</v>
       </c>
       <c r="C72" t="n">
-        <v>-10.6130087989322</v>
+        <v>-1.92476679302634</v>
       </c>
       <c r="D72" t="s">
         <v>9</v>
@@ -2721,10 +2721,10 @@
         <v>80</v>
       </c>
       <c r="B73" t="n">
-        <v>-10.3452385355098</v>
+        <v>49.9929854365494</v>
       </c>
       <c r="C73" t="n">
-        <v>-3.52788930915139</v>
+        <v>4.63580830552108</v>
       </c>
       <c r="D73" t="s">
         <v>6</v>
@@ -2738,10 +2738,10 @@
         <v>81</v>
       </c>
       <c r="B74" t="n">
-        <v>25.2924541885347</v>
+        <v>53.1951081136415</v>
       </c>
       <c r="C74" t="n">
-        <v>-13.0650549278825</v>
+        <v>6.39157442377965</v>
       </c>
       <c r="D74" t="s">
         <v>9</v>
@@ -2755,10 +2755,10 @@
         <v>82</v>
       </c>
       <c r="B75" t="n">
-        <v>36.0570142051036</v>
+        <v>32.2094563367896</v>
       </c>
       <c r="C75" t="n">
-        <v>11.4291863156091</v>
+        <v>28.9596220348134</v>
       </c>
       <c r="D75" t="s">
         <v>9</v>
@@ -2772,10 +2772,10 @@
         <v>83</v>
       </c>
       <c r="B76" t="n">
-        <v>-10.2917307836026</v>
+        <v>51.6878425922282</v>
       </c>
       <c r="C76" t="n">
-        <v>-8.34425048800511</v>
+        <v>3.40895418536022</v>
       </c>
       <c r="D76" t="s">
         <v>9</v>
@@ -2789,10 +2789,10 @@
         <v>84</v>
       </c>
       <c r="B77" t="n">
-        <v>20.596674153004</v>
+        <v>-83.4762066493299</v>
       </c>
       <c r="C77" t="n">
-        <v>12.7838292540613</v>
+        <v>-16.7547100810369</v>
       </c>
       <c r="D77" t="s">
         <v>6</v>
@@ -2806,10 +2806,10 @@
         <v>85</v>
       </c>
       <c r="B78" t="n">
-        <v>-21.5111416157525</v>
+        <v>72.2348759062137</v>
       </c>
       <c r="C78" t="n">
-        <v>4.76846183676285</v>
+        <v>-21.1767586712523</v>
       </c>
       <c r="D78" t="s">
         <v>9</v>
@@ -2823,10 +2823,10 @@
         <v>86</v>
       </c>
       <c r="B79" t="n">
-        <v>-14.1813073902058</v>
+        <v>42.5461357890273</v>
       </c>
       <c r="C79" t="n">
-        <v>-3.61385699289219</v>
+        <v>9.72549623255701</v>
       </c>
       <c r="D79" t="s">
         <v>9</v>
@@ -2840,10 +2840,10 @@
         <v>87</v>
       </c>
       <c r="B80" t="n">
-        <v>23.4872281353531</v>
+        <v>49.6614930736458</v>
       </c>
       <c r="C80" t="n">
-        <v>-27.2580569864548</v>
+        <v>-10.3754609589632</v>
       </c>
       <c r="D80" t="s">
         <v>9</v>
@@ -2857,10 +2857,10 @@
         <v>88</v>
       </c>
       <c r="B81" t="n">
-        <v>4.54629757840062</v>
+        <v>55.3337465714859</v>
       </c>
       <c r="C81" t="n">
-        <v>-11.4282740386242</v>
+        <v>-15.4531768290047</v>
       </c>
       <c r="D81" t="s">
         <v>9</v>
@@ -2874,10 +2874,10 @@
         <v>89</v>
       </c>
       <c r="B82" t="n">
-        <v>-13.7559040795479</v>
+        <v>35.6048585740927</v>
       </c>
       <c r="C82" t="n">
-        <v>13.4745838484717</v>
+        <v>37.3442689450729</v>
       </c>
       <c r="D82" t="s">
         <v>9</v>
@@ -2891,10 +2891,10 @@
         <v>90</v>
       </c>
       <c r="B83" t="n">
-        <v>-7.7965593583892</v>
+        <v>71.4142658852559</v>
       </c>
       <c r="C83" t="n">
-        <v>2.91208957492939</v>
+        <v>-37.6702898522615</v>
       </c>
       <c r="D83" t="s">
         <v>9</v>
@@ -2908,10 +2908,10 @@
         <v>91</v>
       </c>
       <c r="B84" t="n">
-        <v>-34.0416849127084</v>
+        <v>63.5917596407954</v>
       </c>
       <c r="C84" t="n">
-        <v>6.09714373234483</v>
+        <v>-24.5638022117028</v>
       </c>
       <c r="D84" t="s">
         <v>9</v>
@@ -2925,10 +2925,10 @@
         <v>92</v>
       </c>
       <c r="B85" t="n">
-        <v>19.7027929765297</v>
+        <v>69.7010573791958</v>
       </c>
       <c r="C85" t="n">
-        <v>-2.47958221611752</v>
+        <v>-26.267931333221</v>
       </c>
       <c r="D85" t="s">
         <v>9</v>
@@ -2942,10 +2942,10 @@
         <v>93</v>
       </c>
       <c r="B86" t="n">
-        <v>-13.4339073239469</v>
+        <v>41.4441390214823</v>
       </c>
       <c r="C86" t="n">
-        <v>0.787959551078988</v>
+        <v>16.5057999478367</v>
       </c>
       <c r="D86" t="s">
         <v>9</v>
@@ -2959,10 +2959,10 @@
         <v>94</v>
       </c>
       <c r="B87" t="n">
-        <v>-28.2467060330768</v>
+        <v>68.6380971568392</v>
       </c>
       <c r="C87" t="n">
-        <v>15.2727771002069</v>
+        <v>-23.3404037115443</v>
       </c>
       <c r="D87" t="s">
         <v>9</v>
@@ -2976,10 +2976,10 @@
         <v>95</v>
       </c>
       <c r="B88" t="n">
-        <v>16.2015635486313</v>
+        <v>52.4967791531595</v>
       </c>
       <c r="C88" t="n">
-        <v>-19.5558880277463</v>
+        <v>4.28014197942859</v>
       </c>
       <c r="D88" t="s">
         <v>6</v>
@@ -2993,10 +2993,10 @@
         <v>96</v>
       </c>
       <c r="B89" t="n">
-        <v>-1.51745597659375</v>
+        <v>54.9024747195993</v>
       </c>
       <c r="C89" t="n">
-        <v>4.99994829082001</v>
+        <v>-22.5534541926996</v>
       </c>
       <c r="D89" t="s">
         <v>9</v>
@@ -3010,10 +3010,10 @@
         <v>97</v>
       </c>
       <c r="B90" t="n">
-        <v>-2.23665836595608</v>
+        <v>56.8447416328233</v>
       </c>
       <c r="C90" t="n">
-        <v>-23.9930939091689</v>
+        <v>9.1595487264549</v>
       </c>
       <c r="D90" t="s">
         <v>9</v>
@@ -3027,10 +3027,10 @@
         <v>98</v>
       </c>
       <c r="B91" t="n">
-        <v>-11.6707023049276</v>
+        <v>56.8260068747652</v>
       </c>
       <c r="C91" t="n">
-        <v>-15.0904970117789</v>
+        <v>13.8891063744131</v>
       </c>
       <c r="D91" t="s">
         <v>9</v>
@@ -3044,10 +3044,10 @@
         <v>99</v>
       </c>
       <c r="B92" t="n">
-        <v>3.25709127712848</v>
+        <v>-51.3939651746286</v>
       </c>
       <c r="C92" t="n">
-        <v>-13.7897128541154</v>
+        <v>2.76926150659787</v>
       </c>
       <c r="D92" t="s">
         <v>6</v>
@@ -3061,10 +3061,10 @@
         <v>100</v>
       </c>
       <c r="B93" t="n">
-        <v>0.237111696036269</v>
+        <v>67.669192742792</v>
       </c>
       <c r="C93" t="n">
-        <v>-6.18367948882146</v>
+        <v>-18.9176498930096</v>
       </c>
       <c r="D93" t="s">
         <v>9</v>
@@ -3078,10 +3078,10 @@
         <v>101</v>
       </c>
       <c r="B94" t="n">
-        <v>-15.6521851714067</v>
+        <v>64.7715022735082</v>
       </c>
       <c r="C94" t="n">
-        <v>27.2999680544097</v>
+        <v>-14.9027930375309</v>
       </c>
       <c r="D94" t="s">
         <v>6</v>
@@ -3095,10 +3095,10 @@
         <v>102</v>
       </c>
       <c r="B95" t="n">
-        <v>13.4633490960912</v>
+        <v>69.8112484220601</v>
       </c>
       <c r="C95" t="n">
-        <v>1.44900778212286</v>
+        <v>-45.2223384836728</v>
       </c>
       <c r="D95" t="s">
         <v>9</v>
@@ -3112,10 +3112,10 @@
         <v>103</v>
       </c>
       <c r="B96" t="n">
-        <v>-6.33686045009423</v>
+        <v>-64.2452073847132</v>
       </c>
       <c r="C96" t="n">
-        <v>16.5071282531336</v>
+        <v>10.2836049724314</v>
       </c>
       <c r="D96" t="s">
         <v>6</v>
@@ -3129,10 +3129,10 @@
         <v>104</v>
       </c>
       <c r="B97" t="n">
-        <v>-7.3266844842911</v>
+        <v>48.7403728036317</v>
       </c>
       <c r="C97" t="n">
-        <v>-15.5614817996125</v>
+        <v>17.9486590748238</v>
       </c>
       <c r="D97" t="s">
         <v>6</v>
@@ -3146,10 +3146,10 @@
         <v>105</v>
       </c>
       <c r="B98" t="n">
-        <v>-12.4430000738978</v>
+        <v>54.0640730634344</v>
       </c>
       <c r="C98" t="n">
-        <v>-4.00493957955496</v>
+        <v>-9.84633445814579</v>
       </c>
       <c r="D98" t="s">
         <v>9</v>
@@ -3163,10 +3163,10 @@
         <v>106</v>
       </c>
       <c r="B99" t="n">
-        <v>-35.1721640204243</v>
+        <v>48.8901287791977</v>
       </c>
       <c r="C99" t="n">
-        <v>-0.305932068365005</v>
+        <v>20.2098324160267</v>
       </c>
       <c r="D99" t="s">
         <v>9</v>
@@ -3180,10 +3180,10 @@
         <v>107</v>
       </c>
       <c r="B100" t="n">
-        <v>-3.12115563651158</v>
+        <v>51.3959456002673</v>
       </c>
       <c r="C100" t="n">
-        <v>-17.905292097764</v>
+        <v>7.53109335062453</v>
       </c>
       <c r="D100" t="s">
         <v>9</v>
@@ -3197,10 +3197,10 @@
         <v>108</v>
       </c>
       <c r="B101" t="n">
-        <v>28.4571711714733</v>
+        <v>61.9319397617465</v>
       </c>
       <c r="C101" t="n">
-        <v>-5.77681708171577</v>
+        <v>-15.3647714262097</v>
       </c>
       <c r="D101" t="s">
         <v>9</v>
@@ -3214,10 +3214,10 @@
         <v>109</v>
       </c>
       <c r="B102" t="n">
-        <v>-23.6923664120014</v>
+        <v>36.925057155104</v>
       </c>
       <c r="C102" t="n">
-        <v>4.41483979187979</v>
+        <v>48.5132235886377</v>
       </c>
       <c r="D102" t="s">
         <v>9</v>
@@ -3231,10 +3231,10 @@
         <v>110</v>
       </c>
       <c r="B103" t="n">
-        <v>-10.7639412664754</v>
+        <v>52.4946663633184</v>
       </c>
       <c r="C103" t="n">
-        <v>-1.05279363962017</v>
+        <v>-37.4247392974162</v>
       </c>
       <c r="D103" t="s">
         <v>6</v>
@@ -3248,10 +3248,10 @@
         <v>111</v>
       </c>
       <c r="B104" t="n">
-        <v>8.35640383300873</v>
+        <v>64.0039989441702</v>
       </c>
       <c r="C104" t="n">
-        <v>-16.7125155893443</v>
+        <v>-22.2061813370709</v>
       </c>
       <c r="D104" t="s">
         <v>9</v>
@@ -3265,10 +3265,10 @@
         <v>112</v>
       </c>
       <c r="B105" t="n">
-        <v>19.4511607256337</v>
+        <v>-67.7094037715574</v>
       </c>
       <c r="C105" t="n">
-        <v>5.98611339829276</v>
+        <v>-47.5224485726749</v>
       </c>
       <c r="D105" t="s">
         <v>6</v>
@@ -3282,10 +3282,10 @@
         <v>113</v>
       </c>
       <c r="B106" t="n">
-        <v>-13.0769501460017</v>
+        <v>-55.4472367949624</v>
       </c>
       <c r="C106" t="n">
-        <v>7.61670555375101</v>
+        <v>-30.3023334567187</v>
       </c>
       <c r="D106" t="s">
         <v>6</v>
@@ -3299,10 +3299,10 @@
         <v>114</v>
       </c>
       <c r="B107" t="n">
-        <v>-6.59133840923829</v>
+        <v>-45.7072419583264</v>
       </c>
       <c r="C107" t="n">
-        <v>2.88535822893293</v>
+        <v>-54.7861482130549</v>
       </c>
       <c r="D107" t="s">
         <v>6</v>
@@ -3316,10 +3316,10 @@
         <v>115</v>
       </c>
       <c r="B108" t="n">
-        <v>41.5668416927572</v>
+        <v>49.9856348400788</v>
       </c>
       <c r="C108" t="n">
-        <v>1.00083670719163</v>
+        <v>-0.229830678334548</v>
       </c>
       <c r="D108" t="s">
         <v>9</v>
@@ -3333,10 +3333,10 @@
         <v>116</v>
       </c>
       <c r="B109" t="n">
-        <v>20.1426295170576</v>
+        <v>-87.5292466227617</v>
       </c>
       <c r="C109" t="n">
-        <v>0.904081215096171</v>
+        <v>-13.7323304389159</v>
       </c>
       <c r="D109" t="s">
         <v>6</v>
@@ -3350,10 +3350,10 @@
         <v>117</v>
       </c>
       <c r="B110" t="n">
-        <v>-19.9466434431476</v>
+        <v>-56.3739788176243</v>
       </c>
       <c r="C110" t="n">
-        <v>11.1987872342559</v>
+        <v>3.1527028113573</v>
       </c>
       <c r="D110" t="s">
         <v>6</v>
@@ -3367,10 +3367,10 @@
         <v>118</v>
       </c>
       <c r="B111" t="n">
-        <v>5.90925816378751</v>
+        <v>-84.6228542842378</v>
       </c>
       <c r="C111" t="n">
-        <v>-4.98558571077648</v>
+        <v>5.22068628711847</v>
       </c>
       <c r="D111" t="s">
         <v>6</v>
@@ -3384,10 +3384,10 @@
         <v>119</v>
       </c>
       <c r="B112" t="n">
-        <v>-9.87892344538197</v>
+        <v>-52.6517045635291</v>
       </c>
       <c r="C112" t="n">
-        <v>18.7019930930995</v>
+        <v>14.079878635574</v>
       </c>
       <c r="D112" t="s">
         <v>6</v>
@@ -3401,10 +3401,10 @@
         <v>120</v>
       </c>
       <c r="B113" t="n">
-        <v>-21.8088876788848</v>
+        <v>46.9528163301153</v>
       </c>
       <c r="C113" t="n">
-        <v>-22.9086453263141</v>
+        <v>1.55500288008626</v>
       </c>
       <c r="D113" t="s">
         <v>9</v>
@@ -3418,10 +3418,10 @@
         <v>121</v>
       </c>
       <c r="B114" t="n">
-        <v>-25.6415535480124</v>
+        <v>50.4586140626307</v>
       </c>
       <c r="C114" t="n">
-        <v>8.22909373143169</v>
+        <v>23.4640294887354</v>
       </c>
       <c r="D114" t="s">
         <v>9</v>
@@ -3435,10 +3435,10 @@
         <v>122</v>
       </c>
       <c r="B115" t="n">
-        <v>1.70819039464275</v>
+        <v>58.8018642846821</v>
       </c>
       <c r="C115" t="n">
-        <v>1.28441480308368</v>
+        <v>-0.317977008162046</v>
       </c>
       <c r="D115" t="s">
         <v>9</v>
@@ -3452,10 +3452,10 @@
         <v>123</v>
       </c>
       <c r="B116" t="n">
-        <v>-22.1331881084835</v>
+        <v>48.2686384627844</v>
       </c>
       <c r="C116" t="n">
-        <v>-2.25726948409437</v>
+        <v>2.50328789276927</v>
       </c>
       <c r="D116" t="s">
         <v>9</v>
@@ -3469,10 +3469,10 @@
         <v>124</v>
       </c>
       <c r="B117" t="n">
-        <v>-14.4046583649208</v>
+        <v>-47.6635583174125</v>
       </c>
       <c r="C117" t="n">
-        <v>-5.49461898265265</v>
+        <v>-6.17835738966812</v>
       </c>
       <c r="D117" t="s">
         <v>6</v>
@@ -3486,10 +3486,10 @@
         <v>125</v>
       </c>
       <c r="B118" t="n">
-        <v>-23.9683181847131</v>
+        <v>47.1154635178239</v>
       </c>
       <c r="C118" t="n">
-        <v>-31.1436523779297</v>
+        <v>26.0324600979102</v>
       </c>
       <c r="D118" t="s">
         <v>9</v>
@@ -3503,10 +3503,10 @@
         <v>126</v>
       </c>
       <c r="B119" t="n">
-        <v>-4.79903495616081</v>
+        <v>44.4304521476632</v>
       </c>
       <c r="C119" t="n">
-        <v>5.24930987860358</v>
+        <v>2.83214835629623</v>
       </c>
       <c r="D119" t="s">
         <v>9</v>
@@ -3520,10 +3520,10 @@
         <v>127</v>
       </c>
       <c r="B120" t="n">
-        <v>23.0100871768276</v>
+        <v>-58.0178602695103</v>
       </c>
       <c r="C120" t="n">
-        <v>-24.7421633659397</v>
+        <v>-15.921479865082</v>
       </c>
       <c r="D120" t="s">
         <v>6</v>
@@ -3537,10 +3537,10 @@
         <v>128</v>
       </c>
       <c r="B121" t="n">
-        <v>-11.9040710992896</v>
+        <v>-56.8337335514577</v>
       </c>
       <c r="C121" t="n">
-        <v>3.34944560674267</v>
+        <v>-4.63510078571831</v>
       </c>
       <c r="D121" t="s">
         <v>6</v>
@@ -3554,10 +3554,10 @@
         <v>129</v>
       </c>
       <c r="B122" t="n">
-        <v>-3.34532269239941</v>
+        <v>57.7070858905207</v>
       </c>
       <c r="C122" t="n">
-        <v>30.9131465901811</v>
+        <v>-27.5535474878779</v>
       </c>
       <c r="D122" t="s">
         <v>9</v>
@@ -3571,10 +3571,10 @@
         <v>130</v>
       </c>
       <c r="B123" t="n">
-        <v>-2.56108837320891</v>
+        <v>-33.1600859988159</v>
       </c>
       <c r="C123" t="n">
-        <v>0.311160759944318</v>
+        <v>-24.5627676358901</v>
       </c>
       <c r="D123" t="s">
         <v>6</v>
@@ -3588,10 +3588,10 @@
         <v>131</v>
       </c>
       <c r="B124" t="n">
-        <v>9.11428841883174</v>
+        <v>-76.206859664827</v>
       </c>
       <c r="C124" t="n">
-        <v>-5.8027297337073</v>
+        <v>-5.36417313738346</v>
       </c>
       <c r="D124" t="s">
         <v>6</v>
@@ -3605,10 +3605,10 @@
         <v>132</v>
       </c>
       <c r="B125" t="n">
-        <v>-2.04422008117863</v>
+        <v>-55.5268678735318</v>
       </c>
       <c r="C125" t="n">
-        <v>2.49356922756803</v>
+        <v>-18.7485373939884</v>
       </c>
       <c r="D125" t="s">
         <v>6</v>
@@ -3622,10 +3622,10 @@
         <v>133</v>
       </c>
       <c r="B126" t="n">
-        <v>5.22915277733863</v>
+        <v>-29.6045445691351</v>
       </c>
       <c r="C126" t="n">
-        <v>-2.37211555477355</v>
+        <v>-3.29696589014162</v>
       </c>
       <c r="D126" t="s">
         <v>6</v>
@@ -3639,10 +3639,10 @@
         <v>134</v>
       </c>
       <c r="B127" t="n">
-        <v>11.5945337571873</v>
+        <v>-69.6543152368183</v>
       </c>
       <c r="C127" t="n">
-        <v>-8.43231864318185</v>
+        <v>29.8719443384474</v>
       </c>
       <c r="D127" t="s">
         <v>6</v>
@@ -3656,10 +3656,10 @@
         <v>135</v>
       </c>
       <c r="B128" t="n">
-        <v>-1.44462439726168</v>
+        <v>10.3452262649435</v>
       </c>
       <c r="C128" t="n">
-        <v>-7.05487675167302</v>
+        <v>2.13851988061637</v>
       </c>
       <c r="D128" t="s">
         <v>9</v>
@@ -3673,10 +3673,10 @@
         <v>136</v>
       </c>
       <c r="B129" t="n">
-        <v>-15.9865415694566</v>
+        <v>65.5901588431556</v>
       </c>
       <c r="C129" t="n">
-        <v>-14.3631036455919</v>
+        <v>-8.60012989438621</v>
       </c>
       <c r="D129" t="s">
         <v>9</v>
@@ -3690,10 +3690,10 @@
         <v>137</v>
       </c>
       <c r="B130" t="n">
-        <v>-8.28131574550603</v>
+        <v>36.7829512105664</v>
       </c>
       <c r="C130" t="n">
-        <v>-2.60341372224311</v>
+        <v>37.4270504857262</v>
       </c>
       <c r="D130" t="s">
         <v>9</v>
@@ -3707,10 +3707,10 @@
         <v>138</v>
       </c>
       <c r="B131" t="n">
-        <v>-13.3103841566997</v>
+        <v>-66.4751639516886</v>
       </c>
       <c r="C131" t="n">
-        <v>1.08192774145256</v>
+        <v>-42.729622864605</v>
       </c>
       <c r="D131" t="s">
         <v>6</v>
@@ -3724,10 +3724,10 @@
         <v>139</v>
       </c>
       <c r="B132" t="n">
-        <v>28.3661313795341</v>
+        <v>32.3443903000868</v>
       </c>
       <c r="C132" t="n">
-        <v>14.6504422923236</v>
+        <v>-1.96185861867289</v>
       </c>
       <c r="D132" t="s">
         <v>9</v>
@@ -3741,10 +3741,10 @@
         <v>140</v>
       </c>
       <c r="B133" t="n">
-        <v>5.61027230177885</v>
+        <v>-81.3258889463629</v>
       </c>
       <c r="C133" t="n">
-        <v>-7.65094320209683</v>
+        <v>20.1384651688535</v>
       </c>
       <c r="D133" t="s">
         <v>6</v>
@@ -3758,10 +3758,10 @@
         <v>141</v>
       </c>
       <c r="B134" t="n">
-        <v>44.3809851751399</v>
+        <v>39.998029734026</v>
       </c>
       <c r="C134" t="n">
-        <v>0.70142513903898</v>
+        <v>28.7851391391004</v>
       </c>
       <c r="D134" t="s">
         <v>9</v>
@@ -3775,10 +3775,10 @@
         <v>142</v>
       </c>
       <c r="B135" t="n">
-        <v>-26.4296169476108</v>
+        <v>-59.9705630534316</v>
       </c>
       <c r="C135" t="n">
-        <v>10.5012235650566</v>
+        <v>14.9292984116796</v>
       </c>
       <c r="D135" t="s">
         <v>6</v>
@@ -3792,10 +3792,10 @@
         <v>143</v>
       </c>
       <c r="B136" t="n">
-        <v>-16.9483876982058</v>
+        <v>-86.2874827768824</v>
       </c>
       <c r="C136" t="n">
-        <v>4.58555699179009</v>
+        <v>18.3599682069555</v>
       </c>
       <c r="D136" t="s">
         <v>6</v>
@@ -3809,10 +3809,10 @@
         <v>144</v>
       </c>
       <c r="B137" t="n">
-        <v>6.09868823826232</v>
+        <v>-60.0209733649499</v>
       </c>
       <c r="C137" t="n">
-        <v>9.4174937150124</v>
+        <v>1.76303516034804</v>
       </c>
       <c r="D137" t="s">
         <v>6</v>
@@ -3826,10 +3826,10 @@
         <v>145</v>
       </c>
       <c r="B138" t="n">
-        <v>-4.16826173340802</v>
+        <v>-72.9762563358678</v>
       </c>
       <c r="C138" t="n">
-        <v>-1.88860928645865</v>
+        <v>3.80766949585915</v>
       </c>
       <c r="D138" t="s">
         <v>6</v>
@@ -3843,10 +3843,10 @@
         <v>146</v>
       </c>
       <c r="B139" t="n">
-        <v>-8.02850662477977</v>
+        <v>-40.6939091357578</v>
       </c>
       <c r="C139" t="n">
-        <v>-21.0804209335986</v>
+        <v>-16.339175136134</v>
       </c>
       <c r="D139" t="s">
         <v>6</v>
@@ -3860,10 +3860,10 @@
         <v>147</v>
       </c>
       <c r="B140" t="n">
-        <v>6.79368709593756</v>
+        <v>-59.4640792801794</v>
       </c>
       <c r="C140" t="n">
-        <v>-2.8014323501821</v>
+        <v>-3.80320446024598</v>
       </c>
       <c r="D140" t="s">
         <v>6</v>
@@ -3877,10 +3877,10 @@
         <v>148</v>
       </c>
       <c r="B141" t="n">
-        <v>-5.63214439825623</v>
+        <v>-54.5545043987545</v>
       </c>
       <c r="C141" t="n">
-        <v>-6.20059370257996</v>
+        <v>-4.41934795768163</v>
       </c>
       <c r="D141" t="s">
         <v>6</v>
@@ -3894,10 +3894,10 @@
         <v>149</v>
       </c>
       <c r="B142" t="n">
-        <v>6.99456543252333</v>
+        <v>-51.9238060679001</v>
       </c>
       <c r="C142" t="n">
-        <v>15.4050910483094</v>
+        <v>-23.9161802411444</v>
       </c>
       <c r="D142" t="s">
         <v>6</v>
@@ -3911,10 +3911,10 @@
         <v>150</v>
       </c>
       <c r="B143" t="n">
-        <v>-1.34313065843225</v>
+        <v>-18.3797259414198</v>
       </c>
       <c r="C143" t="n">
-        <v>-28.0937566868468</v>
+        <v>-40.9369484399236</v>
       </c>
       <c r="D143" t="s">
         <v>6</v>
@@ -3928,10 +3928,10 @@
         <v>151</v>
       </c>
       <c r="B144" t="n">
-        <v>-4.10083308541435</v>
+        <v>40.9364496436076</v>
       </c>
       <c r="C144" t="n">
-        <v>-18.7697123012993</v>
+        <v>-15.1854636560417</v>
       </c>
       <c r="D144" t="s">
         <v>9</v>
@@ -3945,10 +3945,10 @@
         <v>152</v>
       </c>
       <c r="B145" t="n">
-        <v>-0.742993388223892</v>
+        <v>-65.26784231539</v>
       </c>
       <c r="C145" t="n">
-        <v>-23.6270214992136</v>
+        <v>1.13315651002351</v>
       </c>
       <c r="D145" t="s">
         <v>6</v>
@@ -3962,10 +3962,10 @@
         <v>153</v>
       </c>
       <c r="B146" t="n">
-        <v>-13.6077409954314</v>
+        <v>-47.2321396382505</v>
       </c>
       <c r="C146" t="n">
-        <v>10.94613710473</v>
+        <v>9.51114167765029</v>
       </c>
       <c r="D146" t="s">
         <v>6</v>
@@ -3979,10 +3979,10 @@
         <v>154</v>
       </c>
       <c r="B147" t="n">
-        <v>1.52832701852133</v>
+        <v>-50.2043657353956</v>
       </c>
       <c r="C147" t="n">
-        <v>-18.9947798275031</v>
+        <v>-57.4199079677716</v>
       </c>
       <c r="D147" t="s">
         <v>6</v>
@@ -3996,10 +3996,10 @@
         <v>155</v>
       </c>
       <c r="B148" t="n">
-        <v>8.44227706468024</v>
+        <v>-72.4989676078687</v>
       </c>
       <c r="C148" t="n">
-        <v>-2.28823515182779</v>
+        <v>15.717587417571</v>
       </c>
       <c r="D148" t="s">
         <v>6</v>
@@ -4013,10 +4013,10 @@
         <v>156</v>
       </c>
       <c r="B149" t="n">
-        <v>-1.79775578072726</v>
+        <v>-74.7051692879967</v>
       </c>
       <c r="C149" t="n">
-        <v>0.474976509318277</v>
+        <v>3.45169489381939</v>
       </c>
       <c r="D149" t="s">
         <v>6</v>
@@ -4030,10 +4030,10 @@
         <v>157</v>
       </c>
       <c r="B150" t="n">
-        <v>-16.2805580272147</v>
+        <v>-50.0062814419676</v>
       </c>
       <c r="C150" t="n">
-        <v>-5.9683577658185</v>
+        <v>-4.43433519791392</v>
       </c>
       <c r="D150" t="s">
         <v>6</v>
@@ -4047,10 +4047,10 @@
         <v>158</v>
       </c>
       <c r="B151" t="n">
-        <v>-13.1155800233345</v>
+        <v>-83.4091248743716</v>
       </c>
       <c r="C151" t="n">
-        <v>12.0428383489458</v>
+        <v>-3.37165079869147</v>
       </c>
       <c r="D151" t="s">
         <v>6</v>
@@ -4064,10 +4064,10 @@
         <v>159</v>
       </c>
       <c r="B152" t="n">
-        <v>4.17766518051056</v>
+        <v>-79.914096361051</v>
       </c>
       <c r="C152" t="n">
-        <v>10.6360421872694</v>
+        <v>-10.1788678519691</v>
       </c>
       <c r="D152" t="s">
         <v>6</v>
@@ -4081,10 +4081,10 @@
         <v>160</v>
       </c>
       <c r="B153" t="n">
-        <v>12.1035784791605</v>
+        <v>-45.3764477316646</v>
       </c>
       <c r="C153" t="n">
-        <v>-9.3023854305608</v>
+        <v>-6.37776717401583</v>
       </c>
       <c r="D153" t="s">
         <v>6</v>
@@ -4098,10 +4098,10 @@
         <v>161</v>
       </c>
       <c r="B154" t="n">
-        <v>48.0689253677094</v>
+        <v>31.6726694407315</v>
       </c>
       <c r="C154" t="n">
-        <v>6.24303494071363</v>
+        <v>52.1837506950799</v>
       </c>
       <c r="D154" t="s">
         <v>9</v>
@@ -4115,10 +4115,10 @@
         <v>162</v>
       </c>
       <c r="B155" t="n">
-        <v>19.3042666882553</v>
+        <v>-62.5697619275271</v>
       </c>
       <c r="C155" t="n">
-        <v>-23.6487267581547</v>
+        <v>-6.04101952609537</v>
       </c>
       <c r="D155" t="s">
         <v>6</v>
@@ -4132,10 +4132,10 @@
         <v>163</v>
       </c>
       <c r="B156" t="n">
-        <v>-8.34577455998516</v>
+        <v>-34.0460982761133</v>
       </c>
       <c r="C156" t="n">
-        <v>-4.33620495304878</v>
+        <v>-15.2808745917381</v>
       </c>
       <c r="D156" t="s">
         <v>6</v>
@@ -4149,10 +4149,10 @@
         <v>164</v>
       </c>
       <c r="B157" t="n">
-        <v>-23.4589148788735</v>
+        <v>-44.4862846505315</v>
       </c>
       <c r="C157" t="n">
-        <v>6.7008924813774</v>
+        <v>42.1367920918986</v>
       </c>
       <c r="D157" t="s">
         <v>6</v>
@@ -4166,10 +4166,10 @@
         <v>165</v>
       </c>
       <c r="B158" t="n">
-        <v>-19.0735026076332</v>
+        <v>-40.0623358606674</v>
       </c>
       <c r="C158" t="n">
-        <v>12.9733551373676</v>
+        <v>-6.43867487787796</v>
       </c>
       <c r="D158" t="s">
         <v>6</v>
@@ -4183,10 +4183,10 @@
         <v>166</v>
       </c>
       <c r="B159" t="n">
-        <v>11.2769087512314</v>
+        <v>-60.0798086989785</v>
       </c>
       <c r="C159" t="n">
-        <v>1.31674962793418</v>
+        <v>0.850568936421394</v>
       </c>
       <c r="D159" t="s">
         <v>6</v>
@@ -4200,10 +4200,10 @@
         <v>167</v>
       </c>
       <c r="B160" t="n">
-        <v>-3.06910527395368</v>
+        <v>-11.1232029144943</v>
       </c>
       <c r="C160" t="n">
-        <v>-18.0219357582918</v>
+        <v>-26.5002089809181</v>
       </c>
       <c r="D160" t="s">
         <v>6</v>
@@ -4217,10 +4217,10 @@
         <v>168</v>
       </c>
       <c r="B161" t="n">
-        <v>-0.928357787775094</v>
+        <v>-24.7234978472284</v>
       </c>
       <c r="C161" t="n">
-        <v>30.5601912052269</v>
+        <v>-57.2413345564264</v>
       </c>
       <c r="D161" t="s">
         <v>6</v>
@@ -4234,10 +4234,10 @@
         <v>169</v>
       </c>
       <c r="B162" t="n">
-        <v>-17.3340147962485</v>
+        <v>-79.0339165403614</v>
       </c>
       <c r="C162" t="n">
-        <v>-2.31605578451516</v>
+        <v>27.2869000092436</v>
       </c>
       <c r="D162" t="s">
         <v>6</v>
@@ -4251,10 +4251,10 @@
         <v>170</v>
       </c>
       <c r="B163" t="n">
-        <v>7.82118747757834</v>
+        <v>-20.8802141972327</v>
       </c>
       <c r="C163" t="n">
-        <v>29.1461720853623</v>
+        <v>1.43399498909574</v>
       </c>
       <c r="D163" t="s">
         <v>6</v>
@@ -4268,10 +4268,10 @@
         <v>171</v>
       </c>
       <c r="B164" t="n">
-        <v>-14.9596624078444</v>
+        <v>-39.7449327713264</v>
       </c>
       <c r="C164" t="n">
-        <v>-20.5438335828348</v>
+        <v>-25.3837620543368</v>
       </c>
       <c r="D164" t="s">
         <v>6</v>
@@ -4285,10 +4285,10 @@
         <v>172</v>
       </c>
       <c r="B165" t="n">
-        <v>31.9354995494347</v>
+        <v>-23.0447577911722</v>
       </c>
       <c r="C165" t="n">
-        <v>-29.0679457652934</v>
+        <v>-28.0153696355323</v>
       </c>
       <c r="D165" t="s">
         <v>6</v>
@@ -4302,10 +4302,10 @@
         <v>173</v>
       </c>
       <c r="B166" t="n">
-        <v>13.1986942860985</v>
+        <v>-55.2758740275841</v>
       </c>
       <c r="C166" t="n">
-        <v>-13.4652746901299</v>
+        <v>-3.10481155142775</v>
       </c>
       <c r="D166" t="s">
         <v>6</v>
@@ -4319,10 +4319,10 @@
         <v>174</v>
       </c>
       <c r="B167" t="n">
-        <v>-8.18629643719097</v>
+        <v>-36.7228145097443</v>
       </c>
       <c r="C167" t="n">
-        <v>-29.0201954141073</v>
+        <v>3.72180502364633</v>
       </c>
       <c r="D167" t="s">
         <v>6</v>
@@ -4336,10 +4336,10 @@
         <v>175</v>
       </c>
       <c r="B168" t="n">
-        <v>-12.5649067746245</v>
+        <v>-48.9534252621478</v>
       </c>
       <c r="C168" t="n">
-        <v>-7.11820399493984</v>
+        <v>4.44953372750415</v>
       </c>
       <c r="D168" t="s">
         <v>6</v>
@@ -4353,10 +4353,10 @@
         <v>176</v>
       </c>
       <c r="B169" t="n">
-        <v>14.469933814019</v>
+        <v>-63.8641855953923</v>
       </c>
       <c r="C169" t="n">
-        <v>-3.81906507664781</v>
+        <v>1.39232426404759</v>
       </c>
       <c r="D169" t="s">
         <v>6</v>
@@ -4370,10 +4370,10 @@
         <v>177</v>
       </c>
       <c r="B170" t="n">
-        <v>-5.11117330620273</v>
+        <v>-49.1620012396339</v>
       </c>
       <c r="C170" t="n">
-        <v>42.9565045118303</v>
+        <v>12.1610531702382</v>
       </c>
       <c r="D170" t="s">
         <v>6</v>
@@ -4387,10 +4387,10 @@
         <v>178</v>
       </c>
       <c r="B171" t="n">
-        <v>-21.5093814916047</v>
+        <v>-59.6011032306584</v>
       </c>
       <c r="C171" t="n">
-        <v>14.4131430260338</v>
+        <v>7.23925588444584</v>
       </c>
       <c r="D171" t="s">
         <v>6</v>
@@ -4404,10 +4404,10 @@
         <v>179</v>
       </c>
       <c r="B172" t="n">
-        <v>-20.7169034823724</v>
+        <v>-57.2666094499116</v>
       </c>
       <c r="C172" t="n">
-        <v>8.71877027338823</v>
+        <v>27.3322513279402</v>
       </c>
       <c r="D172" t="s">
         <v>6</v>
@@ -4421,10 +4421,10 @@
         <v>180</v>
       </c>
       <c r="B173" t="n">
-        <v>-16.1008983604498</v>
+        <v>56.0374076962823</v>
       </c>
       <c r="C173" t="n">
-        <v>16.4353602219307</v>
+        <v>23.6804344819617</v>
       </c>
       <c r="D173" t="s">
         <v>9</v>
@@ -4438,10 +4438,10 @@
         <v>181</v>
       </c>
       <c r="B174" t="n">
-        <v>-29.4197312968898</v>
+        <v>21.1467407053755</v>
       </c>
       <c r="C174" t="n">
-        <v>-4.82317626668954</v>
+        <v>-20.0249470414393</v>
       </c>
       <c r="D174" t="s">
         <v>6</v>
@@ -4455,10 +4455,10 @@
         <v>182</v>
       </c>
       <c r="B175" t="n">
-        <v>-16.4374996817118</v>
+        <v>-26.1081449543802</v>
       </c>
       <c r="C175" t="n">
-        <v>3.64386681058325</v>
+        <v>-17.080293423879</v>
       </c>
       <c r="D175" t="s">
         <v>6</v>
@@ -4472,10 +4472,10 @@
         <v>183</v>
       </c>
       <c r="B176" t="n">
-        <v>5.69504159114468</v>
+        <v>-73.7347370092789</v>
       </c>
       <c r="C176" t="n">
-        <v>0.527562722996551</v>
+        <v>-0.523016767379406</v>
       </c>
       <c r="D176" t="s">
         <v>6</v>
@@ -4489,10 +4489,10 @@
         <v>184</v>
       </c>
       <c r="B177" t="n">
-        <v>11.2409525620878</v>
+        <v>-71.3558893184579</v>
       </c>
       <c r="C177" t="n">
-        <v>4.04824813780127</v>
+        <v>-22.0708426407941</v>
       </c>
       <c r="D177" t="s">
         <v>6</v>
@@ -4506,10 +4506,10 @@
         <v>185</v>
       </c>
       <c r="B178" t="n">
-        <v>-0.578830271382066</v>
+        <v>-20.9302206107112</v>
       </c>
       <c r="C178" t="n">
-        <v>-21.3816631185717</v>
+        <v>1.87760587298859</v>
       </c>
       <c r="D178" t="s">
         <v>6</v>
@@ -4523,10 +4523,10 @@
         <v>186</v>
       </c>
       <c r="B179" t="n">
-        <v>7.41709175264916</v>
+        <v>-23.2048267675621</v>
       </c>
       <c r="C179" t="n">
-        <v>30.8279665685807</v>
+        <v>39.3857675358405</v>
       </c>
       <c r="D179" t="s">
         <v>6</v>
@@ -4540,10 +4540,10 @@
         <v>187</v>
       </c>
       <c r="B180" t="n">
-        <v>9.81802960314138</v>
+        <v>57.5311976628256</v>
       </c>
       <c r="C180" t="n">
-        <v>4.5352743075262</v>
+        <v>-27.0756955874672</v>
       </c>
       <c r="D180" t="s">
         <v>9</v>
@@ -4557,10 +4557,10 @@
         <v>188</v>
       </c>
       <c r="B181" t="n">
-        <v>-34.8970731529547</v>
+        <v>-33.1908957319549</v>
       </c>
       <c r="C181" t="n">
-        <v>8.73311437646924</v>
+        <v>21.8983451517434</v>
       </c>
       <c r="D181" t="s">
         <v>6</v>
@@ -4574,10 +4574,10 @@
         <v>189</v>
       </c>
       <c r="B182" t="n">
-        <v>2.58556294128933</v>
+        <v>57.1045472683084</v>
       </c>
       <c r="C182" t="n">
-        <v>15.6760614865759</v>
+        <v>-19.1790528952322</v>
       </c>
       <c r="D182" t="s">
         <v>9</v>
@@ -4591,10 +4591,10 @@
         <v>190</v>
       </c>
       <c r="B183" t="n">
-        <v>2.66569012104583</v>
+        <v>58.0360713188645</v>
       </c>
       <c r="C183" t="n">
-        <v>-4.18884712576226</v>
+        <v>-12.1127717344119</v>
       </c>
       <c r="D183" t="s">
         <v>9</v>
@@ -4608,10 +4608,10 @@
         <v>191</v>
       </c>
       <c r="B184" t="n">
-        <v>-0.147100768285717</v>
+        <v>-64.6927922214275</v>
       </c>
       <c r="C184" t="n">
-        <v>-0.717720487259096</v>
+        <v>31.0952343666759</v>
       </c>
       <c r="D184" t="s">
         <v>6</v>
@@ -4625,10 +4625,10 @@
         <v>192</v>
       </c>
       <c r="B185" t="n">
-        <v>5.8839228257603</v>
+        <v>-96.843742844739</v>
       </c>
       <c r="C185" t="n">
-        <v>7.00063610762925</v>
+        <v>7.63801716192717</v>
       </c>
       <c r="D185" t="s">
         <v>6</v>
@@ -4642,10 +4642,10 @@
         <v>193</v>
       </c>
       <c r="B186" t="n">
-        <v>5.24928080330954</v>
+        <v>-54.2441127401431</v>
       </c>
       <c r="C186" t="n">
-        <v>-3.22978852400934</v>
+        <v>-25.6451995741316</v>
       </c>
       <c r="D186" t="s">
         <v>6</v>
@@ -4659,10 +4659,10 @@
         <v>194</v>
       </c>
       <c r="B187" t="n">
-        <v>-21.8435929221272</v>
+        <v>-78.1984567407726</v>
       </c>
       <c r="C187" t="n">
-        <v>-0.323080705732658</v>
+        <v>2.71683391797406</v>
       </c>
       <c r="D187" t="s">
         <v>6</v>
@@ -4676,10 +4676,10 @@
         <v>195</v>
       </c>
       <c r="B188" t="n">
-        <v>-22.3782707419422</v>
+        <v>53.9826449701186</v>
       </c>
       <c r="C188" t="n">
-        <v>-12.4233912406863</v>
+        <v>-1.2254380097622</v>
       </c>
       <c r="D188" t="s">
         <v>9</v>
@@ -4693,10 +4693,10 @@
         <v>196</v>
       </c>
       <c r="B189" t="n">
-        <v>2.65625136756657</v>
+        <v>-47.1738968220993</v>
       </c>
       <c r="C189" t="n">
-        <v>-6.61094262564351</v>
+        <v>17.8578829050227</v>
       </c>
       <c r="D189" t="s">
         <v>6</v>
@@ -4710,10 +4710,10 @@
         <v>197</v>
       </c>
       <c r="B190" t="n">
-        <v>4.95021007346315</v>
+        <v>57.8114949703631</v>
       </c>
       <c r="C190" t="n">
-        <v>7.09231470072305</v>
+        <v>-12.9763966496306</v>
       </c>
       <c r="D190" t="s">
         <v>9</v>
@@ -4727,10 +4727,10 @@
         <v>198</v>
       </c>
       <c r="B191" t="n">
-        <v>8.61399994083995</v>
+        <v>-78.4235859388464</v>
       </c>
       <c r="C191" t="n">
-        <v>-18.2914897506319</v>
+        <v>-10.0502821796925</v>
       </c>
       <c r="D191" t="s">
         <v>6</v>
@@ -4744,10 +4744,10 @@
         <v>199</v>
       </c>
       <c r="B192" t="n">
-        <v>-13.0158164923235</v>
+        <v>59.8437456978591</v>
       </c>
       <c r="C192" t="n">
-        <v>-22.8239564621242</v>
+        <v>-0.615996354593427</v>
       </c>
       <c r="D192" t="s">
         <v>9</v>
@@ -4761,10 +4761,10 @@
         <v>200</v>
       </c>
       <c r="B193" t="n">
-        <v>5.03805953287724</v>
+        <v>48.5216363070637</v>
       </c>
       <c r="C193" t="n">
-        <v>11.9270282212819</v>
+        <v>-6.0235510852738</v>
       </c>
       <c r="D193" t="s">
         <v>9</v>
@@ -4778,10 +4778,10 @@
         <v>201</v>
       </c>
       <c r="B194" t="n">
-        <v>-7.24808261405374</v>
+        <v>-12.6214627146757</v>
       </c>
       <c r="C194" t="n">
-        <v>9.50691187034063</v>
+        <v>12.6350572654852</v>
       </c>
       <c r="D194" t="s">
         <v>6</v>
@@ -4795,10 +4795,10 @@
         <v>202</v>
       </c>
       <c r="B195" t="n">
-        <v>7.45031401609494</v>
+        <v>-45.6842136012905</v>
       </c>
       <c r="C195" t="n">
-        <v>15.9805177043714</v>
+        <v>-13.3408424407596</v>
       </c>
       <c r="D195" t="s">
         <v>6</v>
@@ -4812,10 +4812,10 @@
         <v>203</v>
       </c>
       <c r="B196" t="n">
-        <v>3.18415867218198</v>
+        <v>64.5094374291874</v>
       </c>
       <c r="C196" t="n">
-        <v>9.42391759508452</v>
+        <v>-14.4946250108136</v>
       </c>
       <c r="D196" t="s">
         <v>9</v>
@@ -4829,10 +4829,10 @@
         <v>204</v>
       </c>
       <c r="B197" t="n">
-        <v>2.37768840590952</v>
+        <v>-50.8198263603602</v>
       </c>
       <c r="C197" t="n">
-        <v>-7.00438591947626</v>
+        <v>10.9031940015413</v>
       </c>
       <c r="D197" t="s">
         <v>6</v>
@@ -4846,10 +4846,10 @@
         <v>205</v>
       </c>
       <c r="B198" t="n">
-        <v>-7.84516048409109</v>
+        <v>-73.423688305023</v>
       </c>
       <c r="C198" t="n">
-        <v>4.84786945150325</v>
+        <v>-18.1777309066529</v>
       </c>
       <c r="D198" t="s">
         <v>6</v>
@@ -4863,10 +4863,10 @@
         <v>206</v>
       </c>
       <c r="B199" t="n">
-        <v>9.65221945066994</v>
+        <v>53.2628648603113</v>
       </c>
       <c r="C199" t="n">
-        <v>36.0450389351474</v>
+        <v>4.7894193401077</v>
       </c>
       <c r="D199" t="s">
         <v>6</v>
@@ -4880,10 +4880,10 @@
         <v>207</v>
       </c>
       <c r="B200" t="n">
-        <v>21.680164059266</v>
+        <v>48.6499914467004</v>
       </c>
       <c r="C200" t="n">
-        <v>-32.713485615549</v>
+        <v>-0.150751348580779</v>
       </c>
       <c r="D200" t="s">
         <v>6</v>
@@ -4897,10 +4897,10 @@
         <v>208</v>
       </c>
       <c r="B201" t="n">
-        <v>-15.0257535029037</v>
+        <v>-54.2093473940441</v>
       </c>
       <c r="C201" t="n">
-        <v>2.72542573524976</v>
+        <v>26.347636719714</v>
       </c>
       <c r="D201" t="s">
         <v>6</v>
@@ -4914,10 +4914,10 @@
         <v>209</v>
       </c>
       <c r="B202" t="n">
-        <v>25.9231186370883</v>
+        <v>55.3800332126416</v>
       </c>
       <c r="C202" t="n">
-        <v>3.12525423232446</v>
+        <v>-3.45066562179821</v>
       </c>
       <c r="D202" t="s">
         <v>9</v>
@@ -4931,10 +4931,10 @@
         <v>210</v>
       </c>
       <c r="B203" t="n">
-        <v>-24.5037816522943</v>
+        <v>47.3736199268162</v>
       </c>
       <c r="C203" t="n">
-        <v>11.3731959694694</v>
+        <v>15.4798910938804</v>
       </c>
       <c r="D203" t="s">
         <v>6</v>
@@ -4948,10 +4948,10 @@
         <v>211</v>
       </c>
       <c r="B204" t="n">
-        <v>9.28149287507147</v>
+        <v>47.3267965795284</v>
       </c>
       <c r="C204" t="n">
-        <v>0.554317893028854</v>
+        <v>2.55676126155572</v>
       </c>
       <c r="D204" t="s">
         <v>9</v>
@@ -4965,10 +4965,10 @@
         <v>212</v>
       </c>
       <c r="B205" t="n">
-        <v>33.6256930541042</v>
+        <v>63.7126498747078</v>
       </c>
       <c r="C205" t="n">
-        <v>0.728835207707252</v>
+        <v>-24.9871161141349</v>
       </c>
       <c r="D205" t="s">
         <v>9</v>
@@ -4982,10 +4982,10 @@
         <v>213</v>
       </c>
       <c r="B206" t="n">
-        <v>-4.890491487617</v>
+        <v>58.6809164860108</v>
       </c>
       <c r="C206" t="n">
-        <v>10.0068986151163</v>
+        <v>-3.6755349400321</v>
       </c>
       <c r="D206" t="s">
         <v>9</v>
@@ -4999,10 +4999,10 @@
         <v>214</v>
       </c>
       <c r="B207" t="n">
-        <v>-16.6279465806864</v>
+        <v>46.0820610529179</v>
       </c>
       <c r="C207" t="n">
-        <v>-5.26200901512107</v>
+        <v>40.9641156860017</v>
       </c>
       <c r="D207" t="s">
         <v>6</v>
@@ -5016,10 +5016,10 @@
         <v>215</v>
       </c>
       <c r="B208" t="n">
-        <v>11.0209402147655</v>
+        <v>56.0941341759166</v>
       </c>
       <c r="C208" t="n">
-        <v>-10.7287454476277</v>
+        <v>-16.4301942414767</v>
       </c>
       <c r="D208" t="s">
         <v>9</v>
@@ -5033,10 +5033,10 @@
         <v>216</v>
       </c>
       <c r="B209" t="n">
-        <v>-19.5298969757955</v>
+        <v>6.89937482723346</v>
       </c>
       <c r="C209" t="n">
-        <v>1.71970681602549</v>
+        <v>-29.3019378416949</v>
       </c>
       <c r="D209" t="s">
         <v>6</v>
@@ -5050,10 +5050,10 @@
         <v>217</v>
       </c>
       <c r="B210" t="n">
-        <v>30.1186456781536</v>
+        <v>1.61980017059938</v>
       </c>
       <c r="C210" t="n">
-        <v>31.5897949328171</v>
+        <v>19.2351027221272</v>
       </c>
       <c r="D210" t="s">
         <v>6</v>
@@ -5067,10 +5067,10 @@
         <v>218</v>
       </c>
       <c r="B211" t="n">
-        <v>-1.49048749228656</v>
+        <v>60.8213256802816</v>
       </c>
       <c r="C211" t="n">
-        <v>-18.0112977715508</v>
+        <v>-21.1725422049021</v>
       </c>
       <c r="D211" t="s">
         <v>9</v>
@@ -5084,10 +5084,10 @@
         <v>219</v>
       </c>
       <c r="B212" t="n">
-        <v>10.9779312152211</v>
+        <v>-46.056070213829</v>
       </c>
       <c r="C212" t="n">
-        <v>-3.510863870971</v>
+        <v>-1.32901986625112</v>
       </c>
       <c r="D212" t="s">
         <v>6</v>
@@ -5101,10 +5101,10 @@
         <v>220</v>
       </c>
       <c r="B213" t="n">
-        <v>-5.02700406855431</v>
+        <v>-82.3639383117606</v>
       </c>
       <c r="C213" t="n">
-        <v>10.0101390638206</v>
+        <v>-10.7566258757069</v>
       </c>
       <c r="D213" t="s">
         <v>6</v>
@@ -5118,10 +5118,10 @@
         <v>221</v>
       </c>
       <c r="B214" t="n">
-        <v>-3.22431823994908</v>
+        <v>-96.2634259854293</v>
       </c>
       <c r="C214" t="n">
-        <v>8.05193886917678</v>
+        <v>-7.21544646658648</v>
       </c>
       <c r="D214" t="s">
         <v>6</v>
@@ -5135,10 +5135,10 @@
         <v>222</v>
       </c>
       <c r="B215" t="n">
-        <v>6.33294401722043</v>
+        <v>62.4138870404492</v>
       </c>
       <c r="C215" t="n">
-        <v>-24.1752997122105</v>
+        <v>14.2481083071988</v>
       </c>
       <c r="D215" t="s">
         <v>9</v>
@@ -5152,10 +5152,10 @@
         <v>223</v>
       </c>
       <c r="B216" t="n">
-        <v>-13.2921444024513</v>
+        <v>-51.5029982545643</v>
       </c>
       <c r="C216" t="n">
-        <v>-16.2482198386702</v>
+        <v>4.39106213946167</v>
       </c>
       <c r="D216" t="s">
         <v>6</v>
@@ -5169,10 +5169,10 @@
         <v>224</v>
       </c>
       <c r="B217" t="n">
-        <v>-39.0765016477957</v>
+        <v>45.7884444302236</v>
       </c>
       <c r="C217" t="n">
-        <v>19.6377492889574</v>
+        <v>40.2536072564093</v>
       </c>
       <c r="D217" t="s">
         <v>9</v>
@@ -5186,10 +5186,10 @@
         <v>225</v>
       </c>
       <c r="B218" t="n">
-        <v>15.4636579415344</v>
+        <v>46.1843383732782</v>
       </c>
       <c r="C218" t="n">
-        <v>-10.8791578836372</v>
+        <v>19.4107954685258</v>
       </c>
       <c r="D218" t="s">
         <v>9</v>
@@ -5203,10 +5203,10 @@
         <v>226</v>
       </c>
       <c r="B219" t="n">
-        <v>11.0415928368684</v>
+        <v>48.9049613028912</v>
       </c>
       <c r="C219" t="n">
-        <v>25.1820973371773</v>
+        <v>-15.979274437173</v>
       </c>
       <c r="D219" t="s">
         <v>9</v>
@@ -5220,10 +5220,10 @@
         <v>227</v>
       </c>
       <c r="B220" t="n">
-        <v>8.86894719187536</v>
+        <v>-55.3277906963384</v>
       </c>
       <c r="C220" t="n">
-        <v>1.35244698730585</v>
+        <v>-33.3012403313197</v>
       </c>
       <c r="D220" t="s">
         <v>9</v>
@@ -5237,10 +5237,10 @@
         <v>228</v>
       </c>
       <c r="B221" t="n">
-        <v>-39.2596049757164</v>
+        <v>57.0874319594935</v>
       </c>
       <c r="C221" t="n">
-        <v>3.30262437068655</v>
+        <v>-2.8740363580439</v>
       </c>
       <c r="D221" t="s">
         <v>9</v>
@@ -5254,10 +5254,10 @@
         <v>229</v>
       </c>
       <c r="B222" t="n">
-        <v>0.304529899951814</v>
+        <v>-59.7646858155158</v>
       </c>
       <c r="C222" t="n">
-        <v>-6.51214110758268</v>
+        <v>-2.19183044488554</v>
       </c>
       <c r="D222" t="s">
         <v>6</v>
@@ -5271,10 +5271,10 @@
         <v>230</v>
       </c>
       <c r="B223" t="n">
-        <v>-10.6642506990637</v>
+        <v>65.1742577955159</v>
       </c>
       <c r="C223" t="n">
-        <v>21.7357552852681</v>
+        <v>-18.2331330178395</v>
       </c>
       <c r="D223" t="s">
         <v>9</v>
@@ -5288,10 +5288,10 @@
         <v>231</v>
       </c>
       <c r="B224" t="n">
-        <v>2.38586980420771</v>
+        <v>-54.4605709971921</v>
       </c>
       <c r="C224" t="n">
-        <v>8.14338412480665</v>
+        <v>10.6447118039383</v>
       </c>
       <c r="D224" t="s">
         <v>6</v>
@@ -5305,10 +5305,10 @@
         <v>232</v>
       </c>
       <c r="B225" t="n">
-        <v>2.34175960483012</v>
+        <v>-90.39841105448</v>
       </c>
       <c r="C225" t="n">
-        <v>-1.80264596399967</v>
+        <v>21.3824386228292</v>
       </c>
       <c r="D225" t="s">
         <v>6</v>
@@ -5322,10 +5322,10 @@
         <v>233</v>
       </c>
       <c r="B226" t="n">
-        <v>9.64212286717618</v>
+        <v>-82.2662586202742</v>
       </c>
       <c r="C226" t="n">
-        <v>-3.89388227920494</v>
+        <v>-2.72027821897141</v>
       </c>
       <c r="D226" t="s">
         <v>6</v>
@@ -5339,10 +5339,10 @@
         <v>234</v>
       </c>
       <c r="B227" t="n">
-        <v>-4.23328605648904</v>
+        <v>-106.734203408474</v>
       </c>
       <c r="C227" t="n">
-        <v>0.798941034133829</v>
+        <v>6.01907971023961</v>
       </c>
       <c r="D227" t="s">
         <v>6</v>
@@ -5356,10 +5356,10 @@
         <v>235</v>
       </c>
       <c r="B228" t="n">
-        <v>5.12467690222389</v>
+        <v>-73.7256505555099</v>
       </c>
       <c r="C228" t="n">
-        <v>-2.69557564358034</v>
+        <v>9.40032765186854</v>
       </c>
       <c r="D228" t="s">
         <v>6</v>
@@ -5373,10 +5373,10 @@
         <v>236</v>
       </c>
       <c r="B229" t="n">
-        <v>-5.79933463784749</v>
+        <v>57.1152951036329</v>
       </c>
       <c r="C229" t="n">
-        <v>-9.02196184273744</v>
+        <v>-15.5122173972923</v>
       </c>
       <c r="D229" t="s">
         <v>9</v>
@@ -5390,10 +5390,10 @@
         <v>237</v>
       </c>
       <c r="B230" t="n">
-        <v>-11.171254581006</v>
+        <v>-71.2991716193707</v>
       </c>
       <c r="C230" t="n">
-        <v>4.2970195845113</v>
+        <v>6.84009682874353</v>
       </c>
       <c r="D230" t="s">
         <v>6</v>
@@ -5407,10 +5407,10 @@
         <v>238</v>
       </c>
       <c r="B231" t="n">
-        <v>-13.3635658563141</v>
+        <v>-68.5580717072015</v>
       </c>
       <c r="C231" t="n">
-        <v>9.17917839003483</v>
+        <v>19.6417354815695</v>
       </c>
       <c r="D231" t="s">
         <v>6</v>
@@ -5424,10 +5424,10 @@
         <v>239</v>
       </c>
       <c r="B232" t="n">
-        <v>1.08173145190011</v>
+        <v>55.3834827959147</v>
       </c>
       <c r="C232" t="n">
-        <v>-33.7187963804339</v>
+        <v>-13.3801086956292</v>
       </c>
       <c r="D232" t="s">
         <v>9</v>
@@ -5441,10 +5441,10 @@
         <v>240</v>
       </c>
       <c r="B233" t="n">
-        <v>-11.5655189894725</v>
+        <v>-49.9399177262646</v>
       </c>
       <c r="C233" t="n">
-        <v>-6.88286583576955</v>
+        <v>-13.9090356626996</v>
       </c>
       <c r="D233" t="s">
         <v>6</v>
@@ -5458,10 +5458,10 @@
         <v>241</v>
       </c>
       <c r="B234" t="n">
-        <v>-19.2612058667917</v>
+        <v>0.543373061510619</v>
       </c>
       <c r="C234" t="n">
-        <v>8.95681708905814</v>
+        <v>57.3800254351356</v>
       </c>
       <c r="D234" t="s">
         <v>6</v>
@@ -5475,10 +5475,10 @@
         <v>242</v>
       </c>
       <c r="B235" t="n">
-        <v>9.08946227457002</v>
+        <v>61.4541580509805</v>
       </c>
       <c r="C235" t="n">
-        <v>23.3491626593891</v>
+        <v>-16.396577012165</v>
       </c>
       <c r="D235" t="s">
         <v>9</v>
@@ -5492,10 +5492,10 @@
         <v>243</v>
       </c>
       <c r="B236" t="n">
-        <v>-9.02123790288753</v>
+        <v>-45.820951617718</v>
       </c>
       <c r="C236" t="n">
-        <v>-2.68474102578238</v>
+        <v>17.2686820679613</v>
       </c>
       <c r="D236" t="s">
         <v>6</v>
@@ -5509,10 +5509,10 @@
         <v>244</v>
       </c>
       <c r="B237" t="n">
-        <v>17.9634174252697</v>
+        <v>69.0728810702591</v>
       </c>
       <c r="C237" t="n">
-        <v>2.92742385158727</v>
+        <v>-27.3922160483973</v>
       </c>
       <c r="D237" t="s">
         <v>9</v>
@@ -5526,10 +5526,10 @@
         <v>245</v>
       </c>
       <c r="B238" t="n">
-        <v>24.9633449762064</v>
+        <v>45.3470876185396</v>
       </c>
       <c r="C238" t="n">
-        <v>15.0265776401016</v>
+        <v>1.84918306875157</v>
       </c>
       <c r="D238" t="s">
         <v>9</v>
@@ -5543,10 +5543,10 @@
         <v>246</v>
       </c>
       <c r="B239" t="n">
-        <v>6.63084892148464</v>
+        <v>-89.5689955246209</v>
       </c>
       <c r="C239" t="n">
-        <v>12.0056413705878</v>
+        <v>-25.5638197479263</v>
       </c>
       <c r="D239" t="s">
         <v>6</v>
@@ -5560,10 +5560,10 @@
         <v>247</v>
       </c>
       <c r="B240" t="n">
-        <v>-17.0943363323532</v>
+        <v>-22.606345529373</v>
       </c>
       <c r="C240" t="n">
-        <v>-27.6114912194384</v>
+        <v>-19.5132778742913</v>
       </c>
       <c r="D240" t="s">
         <v>6</v>
@@ -5577,10 +5577,10 @@
         <v>248</v>
       </c>
       <c r="B241" t="n">
-        <v>2.38522790571802</v>
+        <v>-78.9010402693799</v>
       </c>
       <c r="C241" t="n">
-        <v>7.85194950507335</v>
+        <v>-48.9625861566425</v>
       </c>
       <c r="D241" t="s">
         <v>6</v>
@@ -5594,10 +5594,10 @@
         <v>249</v>
       </c>
       <c r="B242" t="n">
-        <v>-3.26800153227864</v>
+        <v>54.5698936306178</v>
       </c>
       <c r="C242" t="n">
-        <v>-10.7876946656434</v>
+        <v>21.8138014553616</v>
       </c>
       <c r="D242" t="s">
         <v>9</v>
@@ -5611,10 +5611,10 @@
         <v>250</v>
       </c>
       <c r="B243" t="n">
-        <v>-11.2191668221105</v>
+        <v>-26.3766144922665</v>
       </c>
       <c r="C243" t="n">
-        <v>-7.47434806942048</v>
+        <v>-31.7412256594093</v>
       </c>
       <c r="D243" t="s">
         <v>6</v>
@@ -5628,10 +5628,10 @@
         <v>251</v>
       </c>
       <c r="B244" t="n">
-        <v>-28.7527601330841</v>
+        <v>68.85500496218</v>
       </c>
       <c r="C244" t="n">
-        <v>2.67210170313567</v>
+        <v>-23.7786748714144</v>
       </c>
       <c r="D244" t="s">
         <v>9</v>
@@ -5645,10 +5645,10 @@
         <v>252</v>
       </c>
       <c r="B245" t="n">
-        <v>7.23549913536927</v>
+        <v>-79.5486566598563</v>
       </c>
       <c r="C245" t="n">
-        <v>1.75446281107142</v>
+        <v>19.7783972406733</v>
       </c>
       <c r="D245" t="s">
         <v>6</v>
@@ -5662,10 +5662,10 @@
         <v>253</v>
       </c>
       <c r="B246" t="n">
-        <v>-3.78390315309657</v>
+        <v>-74.2239208073675</v>
       </c>
       <c r="C246" t="n">
-        <v>25.3665564329125</v>
+        <v>-10.191168914682</v>
       </c>
       <c r="D246" t="s">
         <v>6</v>
@@ -5679,10 +5679,10 @@
         <v>254</v>
       </c>
       <c r="B247" t="n">
-        <v>-38.8994061837988</v>
+        <v>-36.8435840881289</v>
       </c>
       <c r="C247" t="n">
-        <v>9.23365217226933</v>
+        <v>25.6684039280139</v>
       </c>
       <c r="D247" t="s">
         <v>6</v>
@@ -5696,10 +5696,10 @@
         <v>255</v>
       </c>
       <c r="B248" t="n">
-        <v>-25.8134714209444</v>
+        <v>-36.711686233297</v>
       </c>
       <c r="C248" t="n">
-        <v>-6.1576351601575</v>
+        <v>46.6572648286553</v>
       </c>
       <c r="D248" t="s">
         <v>6</v>
@@ -5713,10 +5713,10 @@
         <v>256</v>
       </c>
       <c r="B249" t="n">
-        <v>-6.94206243559024</v>
+        <v>-56.8255401130971</v>
       </c>
       <c r="C249" t="n">
-        <v>4.76807692569685</v>
+        <v>5.93206580943088</v>
       </c>
       <c r="D249" t="s">
         <v>6</v>
@@ -5730,10 +5730,10 @@
         <v>257</v>
       </c>
       <c r="B250" t="n">
-        <v>-0.326402851507935</v>
+        <v>-83.8453446408669</v>
       </c>
       <c r="C250" t="n">
-        <v>-8.8371532793614</v>
+        <v>1.66116146697021</v>
       </c>
       <c r="D250" t="s">
         <v>6</v>
@@ -5747,10 +5747,10 @@
         <v>258</v>
       </c>
       <c r="B251" t="n">
-        <v>-9.97497337526673</v>
+        <v>-46.077874601122</v>
       </c>
       <c r="C251" t="n">
-        <v>2.42506958105463</v>
+        <v>4.50324238490453</v>
       </c>
       <c r="D251" t="s">
         <v>6</v>
@@ -5764,10 +5764,10 @@
         <v>259</v>
       </c>
       <c r="B252" t="n">
-        <v>-19.6946910461324</v>
+        <v>60.4952018584763</v>
       </c>
       <c r="C252" t="n">
-        <v>-10.9538300065562</v>
+        <v>-3.37181630534062</v>
       </c>
       <c r="D252" t="s">
         <v>9</v>
@@ -5781,10 +5781,10 @@
         <v>260</v>
       </c>
       <c r="B253" t="n">
-        <v>6.28132749655861</v>
+        <v>-72.2667333556448</v>
       </c>
       <c r="C253" t="n">
-        <v>-17.7508580238973</v>
+        <v>-15.8786686682549</v>
       </c>
       <c r="D253" t="s">
         <v>6</v>
@@ -5798,10 +5798,10 @@
         <v>261</v>
       </c>
       <c r="B254" t="n">
-        <v>6.30811268613827</v>
+        <v>-76.9906578407365</v>
       </c>
       <c r="C254" t="n">
-        <v>4.29266100369394</v>
+        <v>0.0696049146900388</v>
       </c>
       <c r="D254" t="s">
         <v>6</v>
@@ -5815,10 +5815,10 @@
         <v>262</v>
       </c>
       <c r="B255" t="n">
-        <v>-3.65760723539687</v>
+        <v>-26.2637213373027</v>
       </c>
       <c r="C255" t="n">
-        <v>39.3498829236561</v>
+        <v>12.5837913036797</v>
       </c>
       <c r="D255" t="s">
         <v>6</v>
@@ -5832,10 +5832,10 @@
         <v>263</v>
       </c>
       <c r="B256" t="n">
-        <v>59.482990591983</v>
+        <v>30.8810541901684</v>
       </c>
       <c r="C256" t="n">
-        <v>-18.7784778894747</v>
+        <v>48.7788456191147</v>
       </c>
       <c r="D256" t="s">
         <v>9</v>
@@ -5849,10 +5849,10 @@
         <v>264</v>
       </c>
       <c r="B257" t="n">
-        <v>-26.422514991271</v>
+        <v>-26.8845640657322</v>
       </c>
       <c r="C257" t="n">
-        <v>5.45023666332688</v>
+        <v>34.5931364618969</v>
       </c>
       <c r="D257" t="s">
         <v>6</v>
@@ -5866,10 +5866,10 @@
         <v>265</v>
       </c>
       <c r="B258" t="n">
-        <v>2.62715818488322</v>
+        <v>47.6910665619246</v>
       </c>
       <c r="C258" t="n">
-        <v>-10.6586619017594</v>
+        <v>-25.5132089345943</v>
       </c>
       <c r="D258" t="s">
         <v>9</v>
@@ -5883,10 +5883,10 @@
         <v>266</v>
       </c>
       <c r="B259" t="n">
-        <v>39.0734302843124</v>
+        <v>42.9528907921407</v>
       </c>
       <c r="C259" t="n">
-        <v>-20.9326449536687</v>
+        <v>-0.352972349704279</v>
       </c>
       <c r="D259" t="s">
         <v>9</v>
@@ -5900,10 +5900,10 @@
         <v>267</v>
       </c>
       <c r="B260" t="n">
-        <v>1.5298048491128</v>
+        <v>68.3109164062922</v>
       </c>
       <c r="C260" t="n">
-        <v>-3.49424239044485</v>
+        <v>-31.6172708985468</v>
       </c>
       <c r="D260" t="s">
         <v>9</v>
@@ -5917,10 +5917,10 @@
         <v>268</v>
       </c>
       <c r="B261" t="n">
-        <v>6.95502195144994</v>
+        <v>59.3892397291414</v>
       </c>
       <c r="C261" t="n">
-        <v>32.7842431655276</v>
+        <v>-24.0784310712236</v>
       </c>
       <c r="D261" t="s">
         <v>9</v>
@@ -5934,10 +5934,10 @@
         <v>269</v>
       </c>
       <c r="B262" t="n">
-        <v>15.1188407195549</v>
+        <v>67.0378265324899</v>
       </c>
       <c r="C262" t="n">
-        <v>-7.50901845743124</v>
+        <v>-27.1889106160913</v>
       </c>
       <c r="D262" t="s">
         <v>9</v>
@@ -5951,10 +5951,10 @@
         <v>270</v>
       </c>
       <c r="B263" t="n">
-        <v>-13.0264651101147</v>
+        <v>57.5087737499019</v>
       </c>
       <c r="C263" t="n">
-        <v>3.39932908617193</v>
+        <v>-19.3199535475092</v>
       </c>
       <c r="D263" t="s">
         <v>6</v>
@@ -5968,10 +5968,10 @@
         <v>271</v>
       </c>
       <c r="B264" t="n">
-        <v>10.5975318238995</v>
+        <v>47.6609794166829</v>
       </c>
       <c r="C264" t="n">
-        <v>-21.4638582666979</v>
+        <v>-2.94036627169904</v>
       </c>
       <c r="D264" t="s">
         <v>9</v>
@@ -5985,10 +5985,10 @@
         <v>272</v>
       </c>
       <c r="B265" t="n">
-        <v>-22.2258453784334</v>
+        <v>45.7688672549906</v>
       </c>
       <c r="C265" t="n">
-        <v>-0.611133557433381</v>
+        <v>11.3105604695717</v>
       </c>
       <c r="D265" t="s">
         <v>9</v>
@@ -6002,10 +6002,10 @@
         <v>273</v>
       </c>
       <c r="B266" t="n">
-        <v>16.3580950415197</v>
+        <v>23.9090811684492</v>
       </c>
       <c r="C266" t="n">
-        <v>31.8574016053331</v>
+        <v>45.4778312744969</v>
       </c>
       <c r="D266" t="s">
         <v>9</v>
@@ -6019,10 +6019,10 @@
         <v>274</v>
       </c>
       <c r="B267" t="n">
-        <v>8.5633275291495</v>
+        <v>-84.0791054611971</v>
       </c>
       <c r="C267" t="n">
-        <v>10.1122900117656</v>
+        <v>-1.78813900940985</v>
       </c>
       <c r="D267" t="s">
         <v>6</v>
@@ -6036,10 +6036,10 @@
         <v>275</v>
       </c>
       <c r="B268" t="n">
-        <v>12.1122135643727</v>
+        <v>26.7398558487309</v>
       </c>
       <c r="C268" t="n">
-        <v>-30.9911578594862</v>
+        <v>28.2030527023043</v>
       </c>
       <c r="D268" t="s">
         <v>9</v>
@@ -6053,10 +6053,10 @@
         <v>276</v>
       </c>
       <c r="B269" t="n">
-        <v>7.2504110138767</v>
+        <v>-68.1453991781206</v>
       </c>
       <c r="C269" t="n">
-        <v>11.2169771780626</v>
+        <v>21.0062433248331</v>
       </c>
       <c r="D269" t="s">
         <v>6</v>
@@ -6070,10 +6070,10 @@
         <v>277</v>
       </c>
       <c r="B270" t="n">
-        <v>6.7507735494413</v>
+        <v>-68.1592281133128</v>
       </c>
       <c r="C270" t="n">
-        <v>-0.145289333521945</v>
+        <v>4.28443036520333</v>
       </c>
       <c r="D270" t="s">
         <v>6</v>
@@ -6087,10 +6087,10 @@
         <v>278</v>
       </c>
       <c r="B271" t="n">
-        <v>-0.531124935424838</v>
+        <v>-32.7952157761251</v>
       </c>
       <c r="C271" t="n">
-        <v>2.02444137193503</v>
+        <v>-18.7544201366734</v>
       </c>
       <c r="D271" t="s">
         <v>6</v>
@@ -6104,10 +6104,10 @@
         <v>279</v>
       </c>
       <c r="B272" t="n">
-        <v>-18.6698872233239</v>
+        <v>-36.6308207732047</v>
       </c>
       <c r="C272" t="n">
-        <v>0.841678466777338</v>
+        <v>21.4856699504551</v>
       </c>
       <c r="D272" t="s">
         <v>6</v>
@@ -6121,10 +6121,10 @@
         <v>280</v>
       </c>
       <c r="B273" t="n">
-        <v>-12.4797426475946</v>
+        <v>25.9707502426877</v>
       </c>
       <c r="C273" t="n">
-        <v>-6.28996721014277</v>
+        <v>-10.3945817036597</v>
       </c>
       <c r="D273" t="s">
         <v>6</v>
@@ -6138,10 +6138,10 @@
         <v>281</v>
       </c>
       <c r="B274" t="n">
-        <v>-27.9883880916763</v>
+        <v>7.14973691359763</v>
       </c>
       <c r="C274" t="n">
-        <v>12.8501684001335</v>
+        <v>22.7936306423171</v>
       </c>
       <c r="D274" t="s">
         <v>9</v>
@@ -6155,10 +6155,10 @@
         <v>282</v>
       </c>
       <c r="B275" t="n">
-        <v>10.5717275546153</v>
+        <v>-73.0181951682301</v>
       </c>
       <c r="C275" t="n">
-        <v>19.1794497068522</v>
+        <v>-4.82209494544913</v>
       </c>
       <c r="D275" t="s">
         <v>6</v>
@@ -6172,10 +6172,10 @@
         <v>283</v>
       </c>
       <c r="B276" t="n">
-        <v>-1.60802745864984</v>
+        <v>-87.7172411966229</v>
       </c>
       <c r="C276" t="n">
-        <v>-6.9717380837275</v>
+        <v>1.19536170456111</v>
       </c>
       <c r="D276" t="s">
         <v>6</v>
@@ -6189,10 +6189,10 @@
         <v>284</v>
       </c>
       <c r="B277" t="n">
-        <v>4.33062809737177</v>
+        <v>66.8539079080182</v>
       </c>
       <c r="C277" t="n">
-        <v>-7.53365130504799</v>
+        <v>-29.3194845817833</v>
       </c>
       <c r="D277" t="s">
         <v>9</v>
@@ -6206,10 +6206,10 @@
         <v>285</v>
       </c>
       <c r="B278" t="n">
-        <v>-0.133268559358006</v>
+        <v>45.2629578209009</v>
       </c>
       <c r="C278" t="n">
-        <v>-25.0357679145865</v>
+        <v>26.9329980769555</v>
       </c>
       <c r="D278" t="s">
         <v>9</v>
@@ -6223,10 +6223,10 @@
         <v>286</v>
       </c>
       <c r="B279" t="n">
-        <v>-3.9549770572367</v>
+        <v>-38.7427117863974</v>
       </c>
       <c r="C279" t="n">
-        <v>13.451076700708</v>
+        <v>12.6729081530848</v>
       </c>
       <c r="D279" t="s">
         <v>6</v>
@@ -6240,10 +6240,10 @@
         <v>287</v>
       </c>
       <c r="B280" t="n">
-        <v>26.177973136397</v>
+        <v>-11.9180389660309</v>
       </c>
       <c r="C280" t="n">
-        <v>29.6209365020779</v>
+        <v>54.7318983943381</v>
       </c>
       <c r="D280" t="s">
         <v>9</v>
@@ -6257,10 +6257,10 @@
         <v>288</v>
       </c>
       <c r="B281" t="n">
-        <v>46.27670739001</v>
+        <v>48.1749711715678</v>
       </c>
       <c r="C281" t="n">
-        <v>15.5929828851756</v>
+        <v>14.7812743243663</v>
       </c>
       <c r="D281" t="s">
         <v>9</v>
@@ -6274,10 +6274,10 @@
         <v>289</v>
       </c>
       <c r="B282" t="n">
-        <v>2.68118153460259</v>
+        <v>47.9752913669206</v>
       </c>
       <c r="C282" t="n">
-        <v>-1.15910291211102</v>
+        <v>8.47186143312394</v>
       </c>
       <c r="D282" t="s">
         <v>9</v>
@@ -6291,10 +6291,10 @@
         <v>290</v>
       </c>
       <c r="B283" t="n">
-        <v>5.56313677641037</v>
+        <v>55.9205458480244</v>
       </c>
       <c r="C283" t="n">
-        <v>30.1525886463593</v>
+        <v>-20.6646806736346</v>
       </c>
       <c r="D283" t="s">
         <v>9</v>
@@ -6308,10 +6308,10 @@
         <v>291</v>
       </c>
       <c r="B284" t="n">
-        <v>-2.53187796529145</v>
+        <v>39.3941315198092</v>
       </c>
       <c r="C284" t="n">
-        <v>-3.07671560418979</v>
+        <v>-7.95549188097765</v>
       </c>
       <c r="D284" t="s">
         <v>9</v>
@@ -6325,10 +6325,10 @@
         <v>292</v>
       </c>
       <c r="B285" t="n">
-        <v>8.31162673402497</v>
+        <v>49.9718137171419</v>
       </c>
       <c r="C285" t="n">
-        <v>38.0642802154289</v>
+        <v>12.2666922576662</v>
       </c>
       <c r="D285" t="s">
         <v>9</v>
@@ -6342,10 +6342,10 @@
         <v>293</v>
       </c>
       <c r="B286" t="n">
-        <v>-19.7605572640245</v>
+        <v>-39.8651737012747</v>
       </c>
       <c r="C286" t="n">
-        <v>6.56783803006536</v>
+        <v>-14.2979933284223</v>
       </c>
       <c r="D286" t="s">
         <v>6</v>
@@ -6359,10 +6359,10 @@
         <v>294</v>
       </c>
       <c r="B287" t="n">
-        <v>-26.5452397991294</v>
+        <v>-38.888961719003</v>
       </c>
       <c r="C287" t="n">
-        <v>2.88232190415212</v>
+        <v>-21.471928942222</v>
       </c>
       <c r="D287" t="s">
         <v>6</v>
@@ -6376,10 +6376,10 @@
         <v>295</v>
       </c>
       <c r="B288" t="n">
-        <v>-2.42091130087758</v>
+        <v>-66.105446911483</v>
       </c>
       <c r="C288" t="n">
-        <v>5.50842977830666</v>
+        <v>-55.7186101952891</v>
       </c>
       <c r="D288" t="s">
         <v>6</v>
@@ -6393,10 +6393,10 @@
         <v>296</v>
       </c>
       <c r="B289" t="n">
-        <v>-6.54702613998075</v>
+        <v>54.87381761792</v>
       </c>
       <c r="C289" t="n">
-        <v>-11.2650324272117</v>
+        <v>12.779052580682</v>
       </c>
       <c r="D289" t="s">
         <v>9</v>
@@ -6410,10 +6410,10 @@
         <v>297</v>
       </c>
       <c r="B290" t="n">
-        <v>-24.1318466844834</v>
+        <v>43.292257482336</v>
       </c>
       <c r="C290" t="n">
-        <v>11.9752851083348</v>
+        <v>-22.9432260941795</v>
       </c>
       <c r="D290" t="s">
         <v>9</v>
@@ -6427,10 +6427,10 @@
         <v>298</v>
       </c>
       <c r="B291" t="n">
-        <v>2.67846450619113</v>
+        <v>48.7660680774623</v>
       </c>
       <c r="C291" t="n">
-        <v>-8.03308488024372</v>
+        <v>6.91196009534521</v>
       </c>
       <c r="D291" t="s">
         <v>9</v>
@@ -6444,10 +6444,10 @@
         <v>299</v>
       </c>
       <c r="B292" t="n">
-        <v>-4.41321374553652</v>
+        <v>44.4311145092508</v>
       </c>
       <c r="C292" t="n">
-        <v>-19.4252970101682</v>
+        <v>23.0024285730133</v>
       </c>
       <c r="D292" t="s">
         <v>9</v>
@@ -6461,10 +6461,10 @@
         <v>300</v>
       </c>
       <c r="B293" t="n">
-        <v>22.8832993442068</v>
+        <v>38.3702609264517</v>
       </c>
       <c r="C293" t="n">
-        <v>-20.7691689428363</v>
+        <v>47.265267248922</v>
       </c>
       <c r="D293" t="s">
         <v>9</v>
@@ -6478,10 +6478,10 @@
         <v>301</v>
       </c>
       <c r="B294" t="n">
-        <v>-1.35178267986328</v>
+        <v>-3.41166469209227</v>
       </c>
       <c r="C294" t="n">
-        <v>4.04329589278415</v>
+        <v>-21.4704468088959</v>
       </c>
       <c r="D294" t="s">
         <v>6</v>
@@ -6495,10 +6495,10 @@
         <v>302</v>
       </c>
       <c r="B295" t="n">
-        <v>4.22158596861241</v>
+        <v>-35.3149094989704</v>
       </c>
       <c r="C295" t="n">
-        <v>-9.90802734776153</v>
+        <v>8.45059394350326</v>
       </c>
       <c r="D295" t="s">
         <v>6</v>
@@ -6512,10 +6512,10 @@
         <v>303</v>
       </c>
       <c r="B296" t="n">
-        <v>10.5486722727852</v>
+        <v>-71.1750172009903</v>
       </c>
       <c r="C296" t="n">
-        <v>-6.61342046938882</v>
+        <v>0.331660759851809</v>
       </c>
       <c r="D296" t="s">
         <v>6</v>
@@ -6529,10 +6529,10 @@
         <v>304</v>
       </c>
       <c r="B297" t="n">
-        <v>-2.30713748555557</v>
+        <v>-90.4962349291415</v>
       </c>
       <c r="C297" t="n">
-        <v>17.6349438906863</v>
+        <v>-15.6570037291234</v>
       </c>
       <c r="D297" t="s">
         <v>6</v>
@@ -6546,10 +6546,10 @@
         <v>305</v>
       </c>
       <c r="B298" t="n">
-        <v>6.69941788510692</v>
+        <v>63.6849487189724</v>
       </c>
       <c r="C298" t="n">
-        <v>-8.91005604387683</v>
+        <v>-7.12812230783174</v>
       </c>
       <c r="D298" t="s">
         <v>9</v>
@@ -6563,10 +6563,10 @@
         <v>306</v>
       </c>
       <c r="B299" t="n">
-        <v>14.8717637224892</v>
+        <v>-80.5131140834976</v>
       </c>
       <c r="C299" t="n">
-        <v>-6.29484690993125</v>
+        <v>-2.63459265731022</v>
       </c>
       <c r="D299" t="s">
         <v>6</v>
@@ -6580,10 +6580,10 @@
         <v>307</v>
       </c>
       <c r="B300" t="n">
-        <v>26.2379980715709</v>
+        <v>41.2654598440242</v>
       </c>
       <c r="C300" t="n">
-        <v>2.5984836577219</v>
+        <v>33.0775715159548</v>
       </c>
       <c r="D300" t="s">
         <v>9</v>
@@ -6597,10 +6597,10 @@
         <v>308</v>
       </c>
       <c r="B301" t="n">
-        <v>-2.06675703761214</v>
+        <v>16.6230331261877</v>
       </c>
       <c r="C301" t="n">
-        <v>-14.1568481082305</v>
+        <v>-32.6156685957097</v>
       </c>
       <c r="D301" t="s">
         <v>6</v>
@@ -6614,10 +6614,10 @@
         <v>309</v>
       </c>
       <c r="B302" t="n">
-        <v>-1.06443386326514</v>
+        <v>53.0111501612726</v>
       </c>
       <c r="C302" t="n">
-        <v>10.1048759307477</v>
+        <v>10.9472070942722</v>
       </c>
       <c r="D302" t="s">
         <v>9</v>
@@ -6631,10 +6631,10 @@
         <v>310</v>
       </c>
       <c r="B303" t="n">
-        <v>-14.2475718873916</v>
+        <v>54.4893275790551</v>
       </c>
       <c r="C303" t="n">
-        <v>-9.86024332751161</v>
+        <v>-4.03350836659876</v>
       </c>
       <c r="D303" t="s">
         <v>9</v>
@@ -6648,10 +6648,10 @@
         <v>311</v>
       </c>
       <c r="B304" t="n">
-        <v>33.1094611878398</v>
+        <v>54.4088935093008</v>
       </c>
       <c r="C304" t="n">
-        <v>-11.6303412852648</v>
+        <v>-5.75902845148566</v>
       </c>
       <c r="D304" t="s">
         <v>9</v>
@@ -6665,10 +6665,10 @@
         <v>312</v>
       </c>
       <c r="B305" t="n">
-        <v>25.6228556185148</v>
+        <v>-45.5450146444032</v>
       </c>
       <c r="C305" t="n">
-        <v>-21.6480226016966</v>
+        <v>-35.3503224982223</v>
       </c>
       <c r="D305" t="s">
         <v>6</v>
@@ -6682,10 +6682,10 @@
         <v>313</v>
       </c>
       <c r="B306" t="n">
-        <v>20.2616760870225</v>
+        <v>41.1891608043883</v>
       </c>
       <c r="C306" t="n">
-        <v>-23.0195723911822</v>
+        <v>20.3578435225542</v>
       </c>
       <c r="D306" t="s">
         <v>9</v>
@@ -6699,10 +6699,10 @@
         <v>314</v>
       </c>
       <c r="B307" t="n">
-        <v>-0.791701347196712</v>
+        <v>-64.2246093329293</v>
       </c>
       <c r="C307" t="n">
-        <v>7.31562815427343</v>
+        <v>-7.77063573616571</v>
       </c>
       <c r="D307" t="s">
         <v>6</v>
@@ -6716,10 +6716,10 @@
         <v>315</v>
       </c>
       <c r="B308" t="n">
-        <v>-5.68038561240842</v>
+        <v>-81.7587048242678</v>
       </c>
       <c r="C308" t="n">
-        <v>-0.239933080279871</v>
+        <v>24.9111907006085</v>
       </c>
       <c r="D308" t="s">
         <v>6</v>
@@ -6733,10 +6733,10 @@
         <v>316</v>
       </c>
       <c r="B309" t="n">
-        <v>-11.5954160960392</v>
+        <v>65.3510695430464</v>
       </c>
       <c r="C309" t="n">
-        <v>10.8545297358051</v>
+        <v>-11.205182581048</v>
       </c>
       <c r="D309" t="s">
         <v>9</v>
@@ -6750,10 +6750,10 @@
         <v>317</v>
       </c>
       <c r="B310" t="n">
-        <v>4.74376523785159</v>
+        <v>53.8504875607027</v>
       </c>
       <c r="C310" t="n">
-        <v>7.85059432071263</v>
+        <v>-8.55891963855726</v>
       </c>
       <c r="D310" t="s">
         <v>9</v>
@@ -6767,10 +6767,10 @@
         <v>318</v>
       </c>
       <c r="B311" t="n">
-        <v>-0.31206467456009</v>
+        <v>-71.3079617832848</v>
       </c>
       <c r="C311" t="n">
-        <v>4.10773028291202</v>
+        <v>3.63992884339906</v>
       </c>
       <c r="D311" t="s">
         <v>6</v>
@@ -6784,10 +6784,10 @@
         <v>319</v>
       </c>
       <c r="B312" t="n">
-        <v>-4.25343658185179</v>
+        <v>-32.9659291859639</v>
       </c>
       <c r="C312" t="n">
-        <v>-6.34357999466472</v>
+        <v>24.9781895474999</v>
       </c>
       <c r="D312" t="s">
         <v>6</v>
@@ -6801,10 +6801,10 @@
         <v>320</v>
       </c>
       <c r="B313" t="n">
-        <v>0.246670768797401</v>
+        <v>-94.5529494925592</v>
       </c>
       <c r="C313" t="n">
-        <v>2.60693935644106</v>
+        <v>-13.7137730961937</v>
       </c>
       <c r="D313" t="s">
         <v>6</v>
@@ -6818,10 +6818,10 @@
         <v>321</v>
       </c>
       <c r="B314" t="n">
-        <v>13.6113078133575</v>
+        <v>58.7111888532057</v>
       </c>
       <c r="C314" t="n">
-        <v>36.0735605082724</v>
+        <v>-29.8911178289997</v>
       </c>
       <c r="D314" t="s">
         <v>9</v>
@@ -6835,10 +6835,10 @@
         <v>322</v>
       </c>
       <c r="B315" t="n">
-        <v>5.34655114617685</v>
+        <v>-81.5114546359805</v>
       </c>
       <c r="C315" t="n">
-        <v>-7.12980917000455</v>
+        <v>0.525348116105071</v>
       </c>
       <c r="D315" t="s">
         <v>6</v>
@@ -6852,10 +6852,10 @@
         <v>323</v>
       </c>
       <c r="B316" t="n">
-        <v>30.684546062451</v>
+        <v>-76.3962426921082</v>
       </c>
       <c r="C316" t="n">
-        <v>-26.9967331307787</v>
+        <v>8.2785209789069</v>
       </c>
       <c r="D316" t="s">
         <v>6</v>
@@ -6869,10 +6869,10 @@
         <v>324</v>
       </c>
       <c r="B317" t="n">
-        <v>10.1889375170964</v>
+        <v>-56.2544941270909</v>
       </c>
       <c r="C317" t="n">
-        <v>-4.25113725009436</v>
+        <v>17.4822164924647</v>
       </c>
       <c r="D317" t="s">
         <v>6</v>
@@ -6886,10 +6886,10 @@
         <v>325</v>
       </c>
       <c r="B318" t="n">
-        <v>15.7924970291137</v>
+        <v>-77.9232031440135</v>
       </c>
       <c r="C318" t="n">
-        <v>26.367938517578</v>
+        <v>1.96500465282823</v>
       </c>
       <c r="D318" t="s">
         <v>6</v>
@@ -6903,10 +6903,10 @@
         <v>326</v>
       </c>
       <c r="B319" t="n">
-        <v>8.7560384962251</v>
+        <v>-75.0258411188221</v>
       </c>
       <c r="C319" t="n">
-        <v>-1.04487607046482</v>
+        <v>9.89880087058419</v>
       </c>
       <c r="D319" t="s">
         <v>6</v>
@@ -6920,10 +6920,10 @@
         <v>327</v>
       </c>
       <c r="B320" t="n">
-        <v>21.9716711158158</v>
+        <v>64.6946363295611</v>
       </c>
       <c r="C320" t="n">
-        <v>30.6796609314534</v>
+        <v>-25.2977368716432</v>
       </c>
       <c r="D320" t="s">
         <v>9</v>
@@ -6937,10 +6937,10 @@
         <v>328</v>
       </c>
       <c r="B321" t="n">
-        <v>-2.73554403253436</v>
+        <v>50.7866289243534</v>
       </c>
       <c r="C321" t="n">
-        <v>40.8114146867356</v>
+        <v>-8.58498611903118</v>
       </c>
       <c r="D321" t="s">
         <v>9</v>
@@ -6954,10 +6954,10 @@
         <v>329</v>
       </c>
       <c r="B322" t="n">
-        <v>-33.7799400485128</v>
+        <v>50.7215044771669</v>
       </c>
       <c r="C322" t="n">
-        <v>1.22558867557488</v>
+        <v>16.2054128220755</v>
       </c>
       <c r="D322" t="s">
         <v>9</v>
@@ -6971,10 +6971,10 @@
         <v>330</v>
       </c>
       <c r="B323" t="n">
-        <v>5.72283675597963</v>
+        <v>59.8816434131423</v>
       </c>
       <c r="C323" t="n">
-        <v>-9.97231844132304</v>
+        <v>7.86073377048422</v>
       </c>
       <c r="D323" t="s">
         <v>9</v>
@@ -6988,10 +6988,10 @@
         <v>331</v>
       </c>
       <c r="B324" t="n">
-        <v>26.2289147208908</v>
+        <v>44.8746804081683</v>
       </c>
       <c r="C324" t="n">
-        <v>32.4820557046051</v>
+        <v>23.3966739937113</v>
       </c>
       <c r="D324" t="s">
         <v>9</v>
@@ -7005,10 +7005,10 @@
         <v>332</v>
       </c>
       <c r="B325" t="n">
-        <v>-20.8998582486543</v>
+        <v>-22.6239670322424</v>
       </c>
       <c r="C325" t="n">
-        <v>-5.8099685195118</v>
+        <v>-30.9108465376567</v>
       </c>
       <c r="D325" t="s">
         <v>6</v>
@@ -7022,10 +7022,10 @@
         <v>333</v>
       </c>
       <c r="B326" t="n">
-        <v>25.738311436302</v>
+        <v>-10.0474767911235</v>
       </c>
       <c r="C326" t="n">
-        <v>26.3694761520987</v>
+        <v>-5.59534323196605</v>
       </c>
       <c r="D326" t="s">
         <v>6</v>
@@ -7039,10 +7039,10 @@
         <v>334</v>
       </c>
       <c r="B327" t="n">
-        <v>-5.99152635707659</v>
+        <v>-49.8129422875158</v>
       </c>
       <c r="C327" t="n">
-        <v>-3.3860882540514</v>
+        <v>-33.3108559848411</v>
       </c>
       <c r="D327" t="s">
         <v>6</v>
@@ -7056,10 +7056,10 @@
         <v>335</v>
       </c>
       <c r="B328" t="n">
-        <v>-26.411241194017</v>
+        <v>23.0590462093092</v>
       </c>
       <c r="C328" t="n">
-        <v>3.76476773941664</v>
+        <v>37.0879042736147</v>
       </c>
       <c r="D328" t="s">
         <v>9</v>
@@ -7073,10 +7073,10 @@
         <v>336</v>
       </c>
       <c r="B329" t="n">
-        <v>-38.3082935228273</v>
+        <v>65.0520573355147</v>
       </c>
       <c r="C329" t="n">
-        <v>-1.11668342589848</v>
+        <v>-16.1035253324578</v>
       </c>
       <c r="D329" t="s">
         <v>9</v>
@@ -7090,10 +7090,10 @@
         <v>337</v>
       </c>
       <c r="B330" t="n">
-        <v>-14.2260728511367</v>
+        <v>52.7471348576144</v>
       </c>
       <c r="C330" t="n">
-        <v>-6.95226645193798</v>
+        <v>-10.0791377314652</v>
       </c>
       <c r="D330" t="s">
         <v>9</v>
@@ -7107,10 +7107,10 @@
         <v>338</v>
       </c>
       <c r="B331" t="n">
-        <v>-0.411804314358091</v>
+        <v>-36.4215381304193</v>
       </c>
       <c r="C331" t="n">
-        <v>-8.444629845391</v>
+        <v>-8.57547069099639</v>
       </c>
       <c r="D331" t="s">
         <v>6</v>
@@ -7124,10 +7124,10 @@
         <v>339</v>
       </c>
       <c r="B332" t="n">
-        <v>2.03490788428715</v>
+        <v>-16.3811114294594</v>
       </c>
       <c r="C332" t="n">
-        <v>-18.1896482697004</v>
+        <v>-14.0791930574096</v>
       </c>
       <c r="D332" t="s">
         <v>6</v>
@@ -7141,10 +7141,10 @@
         <v>340</v>
       </c>
       <c r="B333" t="n">
-        <v>-17.8137617549662</v>
+        <v>-49.9862425927494</v>
       </c>
       <c r="C333" t="n">
-        <v>-5.28984822548302</v>
+        <v>30.0423519399335</v>
       </c>
       <c r="D333" t="s">
         <v>6</v>
@@ -7158,10 +7158,10 @@
         <v>341</v>
       </c>
       <c r="B334" t="n">
-        <v>33.0907318936434</v>
+        <v>33.7477366986556</v>
       </c>
       <c r="C334" t="n">
-        <v>7.16637216481043</v>
+        <v>57.7784873926874</v>
       </c>
       <c r="D334" t="s">
         <v>9</v>
@@ -7175,10 +7175,10 @@
         <v>342</v>
       </c>
       <c r="B335" t="n">
-        <v>7.67212108438406</v>
+        <v>67.7607431181038</v>
       </c>
       <c r="C335" t="n">
-        <v>-13.0444749693642</v>
+        <v>-6.12635239670288</v>
       </c>
       <c r="D335" t="s">
         <v>9</v>
@@ -7192,10 +7192,10 @@
         <v>343</v>
       </c>
       <c r="B336" t="n">
-        <v>0.124393178056378</v>
+        <v>17.7175310392346</v>
       </c>
       <c r="C336" t="n">
-        <v>22.3409169090845</v>
+        <v>-40.0207887667665</v>
       </c>
       <c r="D336" t="s">
         <v>9</v>
@@ -7209,10 +7209,10 @@
         <v>344</v>
       </c>
       <c r="B337" t="n">
-        <v>0.762360033740195</v>
+        <v>51.5778958227844</v>
       </c>
       <c r="C337" t="n">
-        <v>9.03058038295697</v>
+        <v>13.4088871323357</v>
       </c>
       <c r="D337" t="s">
         <v>9</v>
@@ -7226,10 +7226,10 @@
         <v>345</v>
       </c>
       <c r="B338" t="n">
-        <v>-17.5503532993996</v>
+        <v>34.3139999380808</v>
       </c>
       <c r="C338" t="n">
-        <v>-22.8773455955788</v>
+        <v>30.0498890517624</v>
       </c>
       <c r="D338" t="s">
         <v>9</v>
@@ -7243,10 +7243,10 @@
         <v>346</v>
       </c>
       <c r="B339" t="n">
-        <v>-17.709705376794</v>
+        <v>42.1565454317211</v>
       </c>
       <c r="C339" t="n">
-        <v>10.103636730746</v>
+        <v>35.2138505519464</v>
       </c>
       <c r="D339" t="s">
         <v>9</v>
@@ -7260,10 +7260,10 @@
         <v>347</v>
       </c>
       <c r="B340" t="n">
-        <v>14.2067756279817</v>
+        <v>59.4131073228739</v>
       </c>
       <c r="C340" t="n">
-        <v>-0.574325464992343</v>
+        <v>-29.0436750140214</v>
       </c>
       <c r="D340" t="s">
         <v>9</v>
@@ -7277,10 +7277,10 @@
         <v>348</v>
       </c>
       <c r="B341" t="n">
-        <v>18.3978674990098</v>
+        <v>43.9783169728983</v>
       </c>
       <c r="C341" t="n">
-        <v>30.6377728884236</v>
+        <v>17.3909351922722</v>
       </c>
       <c r="D341" t="s">
         <v>9</v>
@@ -7294,10 +7294,10 @@
         <v>349</v>
       </c>
       <c r="B342" t="n">
-        <v>3.12580834337767</v>
+        <v>70.0677820711155</v>
       </c>
       <c r="C342" t="n">
-        <v>-18.1646567125368</v>
+        <v>-26.7661028132413</v>
       </c>
       <c r="D342" t="s">
         <v>9</v>
@@ -7311,10 +7311,10 @@
         <v>350</v>
       </c>
       <c r="B343" t="n">
-        <v>22.9313601083805</v>
+        <v>53.5527036300064</v>
       </c>
       <c r="C343" t="n">
-        <v>0.854402545555258</v>
+        <v>19.4297306050305</v>
       </c>
       <c r="D343" t="s">
         <v>9</v>
@@ -7328,10 +7328,10 @@
         <v>351</v>
       </c>
       <c r="B344" t="n">
-        <v>14.4234819950259</v>
+        <v>-45.6673422595097</v>
       </c>
       <c r="C344" t="n">
-        <v>-38.719173618103</v>
+        <v>3.47620962165905</v>
       </c>
       <c r="D344" t="s">
         <v>6</v>
@@ -7345,10 +7345,10 @@
         <v>352</v>
       </c>
       <c r="B345" t="n">
-        <v>0.289538844457129</v>
+        <v>70.2054572598703</v>
       </c>
       <c r="C345" t="n">
-        <v>13.9310633934933</v>
+        <v>-18.7779614497897</v>
       </c>
       <c r="D345" t="s">
         <v>9</v>
@@ -7362,10 +7362,10 @@
         <v>353</v>
       </c>
       <c r="B346" t="n">
-        <v>-38.3129844725048</v>
+        <v>32.1204770492286</v>
       </c>
       <c r="C346" t="n">
-        <v>0.847907428387818</v>
+        <v>59.7851870352095</v>
       </c>
       <c r="D346" t="s">
         <v>9</v>
@@ -7379,10 +7379,10 @@
         <v>354</v>
       </c>
       <c r="B347" t="n">
-        <v>23.2627311828692</v>
+        <v>52.3438970429992</v>
       </c>
       <c r="C347" t="n">
-        <v>-28.0519384415763</v>
+        <v>8.03995617703252</v>
       </c>
       <c r="D347" t="s">
         <v>9</v>
@@ -7396,10 +7396,10 @@
         <v>355</v>
       </c>
       <c r="B348" t="n">
-        <v>-14.1370830307924</v>
+        <v>-21.3010464121701</v>
       </c>
       <c r="C348" t="n">
-        <v>2.09535177829755</v>
+        <v>-13.1786147465277</v>
       </c>
       <c r="D348" t="s">
         <v>6</v>
@@ -7413,10 +7413,10 @@
         <v>356</v>
       </c>
       <c r="B349" t="n">
-        <v>1.60308316549192</v>
+        <v>37.0923295740488</v>
       </c>
       <c r="C349" t="n">
-        <v>-33.586698896712</v>
+        <v>22.9780743549053</v>
       </c>
       <c r="D349" t="s">
         <v>9</v>
@@ -7430,10 +7430,10 @@
         <v>357</v>
       </c>
       <c r="B350" t="n">
-        <v>-20.434956193783</v>
+        <v>47.9395630810649</v>
       </c>
       <c r="C350" t="n">
-        <v>-1.76264955574286</v>
+        <v>1.98690016348619</v>
       </c>
       <c r="D350" t="s">
         <v>9</v>
@@ -7447,10 +7447,10 @@
         <v>358</v>
       </c>
       <c r="B351" t="n">
-        <v>-5.48910279503201</v>
+        <v>61.9155188047923</v>
       </c>
       <c r="C351" t="n">
-        <v>-9.49629395807817</v>
+        <v>-14.7115482531146</v>
       </c>
       <c r="D351" t="s">
         <v>9</v>
@@ -7464,10 +7464,10 @@
         <v>359</v>
       </c>
       <c r="B352" t="n">
-        <v>-2.16146971772633</v>
+        <v>-67.8584357585625</v>
       </c>
       <c r="C352" t="n">
-        <v>-9.01551013336937</v>
+        <v>3.02823886634719</v>
       </c>
       <c r="D352" t="s">
         <v>6</v>
@@ -7481,10 +7481,10 @@
         <v>360</v>
       </c>
       <c r="B353" t="n">
-        <v>10.3858171301346</v>
+        <v>-62.4100000480733</v>
       </c>
       <c r="C353" t="n">
-        <v>-24.854811751743</v>
+        <v>12.4402152919638</v>
       </c>
       <c r="D353" t="s">
         <v>6</v>
@@ -7498,10 +7498,10 @@
         <v>361</v>
       </c>
       <c r="B354" t="n">
-        <v>-1.95809255372978</v>
+        <v>61.8996609438276</v>
       </c>
       <c r="C354" t="n">
-        <v>-13.9298200457915</v>
+        <v>1.83964221541137</v>
       </c>
       <c r="D354" t="s">
         <v>9</v>
@@ -7515,10 +7515,10 @@
         <v>362</v>
       </c>
       <c r="B355" t="n">
-        <v>14.8730596203018</v>
+        <v>-82.9976321766557</v>
       </c>
       <c r="C355" t="n">
-        <v>7.71211684555301</v>
+        <v>5.28937310858274</v>
       </c>
       <c r="D355" t="s">
         <v>6</v>
@@ -7532,10 +7532,10 @@
         <v>363</v>
       </c>
       <c r="B356" t="n">
-        <v>-3.08413180737183</v>
+        <v>50.8404051148273</v>
       </c>
       <c r="C356" t="n">
-        <v>-4.8145373912327</v>
+        <v>4.98677586572759</v>
       </c>
       <c r="D356" t="s">
         <v>9</v>
@@ -7549,10 +7549,10 @@
         <v>364</v>
       </c>
       <c r="B357" t="n">
-        <v>-13.1419008071863</v>
+        <v>0.940904894812721</v>
       </c>
       <c r="C357" t="n">
-        <v>1.26101515733174</v>
+        <v>-19.268864018678</v>
       </c>
       <c r="D357" t="s">
         <v>6</v>
@@ -7566,10 +7566,10 @@
         <v>365</v>
       </c>
       <c r="B358" t="n">
-        <v>-13.2098918240109</v>
+        <v>50.0792657396265</v>
       </c>
       <c r="C358" t="n">
-        <v>4.84516973237486</v>
+        <v>-19.3571172243795</v>
       </c>
       <c r="D358" t="s">
         <v>9</v>
@@ -7583,10 +7583,10 @@
         <v>366</v>
       </c>
       <c r="B359" t="n">
-        <v>7.82879674207452</v>
+        <v>40.2474818300673</v>
       </c>
       <c r="C359" t="n">
-        <v>-42.7160199911585</v>
+        <v>25.4496462813819</v>
       </c>
       <c r="D359" t="s">
         <v>9</v>
@@ -7600,10 +7600,10 @@
         <v>367</v>
       </c>
       <c r="B360" t="n">
-        <v>22.7533627412235</v>
+        <v>-93.2007558423356</v>
       </c>
       <c r="C360" t="n">
-        <v>24.5318454970888</v>
+        <v>-37.8516495690866</v>
       </c>
       <c r="D360" t="s">
         <v>6</v>
@@ -7617,10 +7617,10 @@
         <v>368</v>
       </c>
       <c r="B361" t="n">
-        <v>14.649857943532</v>
+        <v>9.77139062738482</v>
       </c>
       <c r="C361" t="n">
-        <v>-14.1022275230918</v>
+        <v>11.8829803468007</v>
       </c>
       <c r="D361" t="s">
         <v>6</v>
@@ -7634,10 +7634,10 @@
         <v>369</v>
       </c>
       <c r="B362" t="n">
-        <v>-9.36305444745315</v>
+        <v>-73.7063659391619</v>
       </c>
       <c r="C362" t="n">
-        <v>-3.87352899565048</v>
+        <v>-0.873476900239999</v>
       </c>
       <c r="D362" t="s">
         <v>6</v>
@@ -7651,10 +7651,10 @@
         <v>370</v>
       </c>
       <c r="B363" t="n">
-        <v>14.88260537768</v>
+        <v>-50.898729868149</v>
       </c>
       <c r="C363" t="n">
-        <v>-6.92463041487231</v>
+        <v>-19.6041714026505</v>
       </c>
       <c r="D363" t="s">
         <v>6</v>
@@ -7668,10 +7668,10 @@
         <v>371</v>
       </c>
       <c r="B364" t="n">
-        <v>33.0769597498723</v>
+        <v>47.8667253595258</v>
       </c>
       <c r="C364" t="n">
-        <v>21.54399408869</v>
+        <v>1.82172058906323</v>
       </c>
       <c r="D364" t="s">
         <v>9</v>
@@ -7685,10 +7685,10 @@
         <v>372</v>
       </c>
       <c r="B365" t="n">
-        <v>-13.5323227848568</v>
+        <v>43.6425974661506</v>
       </c>
       <c r="C365" t="n">
-        <v>-5.81619142133997</v>
+        <v>20.069851210581</v>
       </c>
       <c r="D365" t="s">
         <v>9</v>
@@ -7702,10 +7702,10 @@
         <v>373</v>
       </c>
       <c r="B366" t="n">
-        <v>-6.5453944913219</v>
+        <v>-53.9441319631353</v>
       </c>
       <c r="C366" t="n">
-        <v>-9.99897497218557</v>
+        <v>-25.5591654481447</v>
       </c>
       <c r="D366" t="s">
         <v>6</v>
@@ -7719,10 +7719,10 @@
         <v>374</v>
       </c>
       <c r="B367" t="n">
-        <v>-10.9268435732603</v>
+        <v>62.3129450989502</v>
       </c>
       <c r="C367" t="n">
-        <v>-9.15818350464652</v>
+        <v>-19.6063094470279</v>
       </c>
       <c r="D367" t="s">
         <v>9</v>
@@ -7736,10 +7736,10 @@
         <v>375</v>
       </c>
       <c r="B368" t="n">
-        <v>-2.06775939380644</v>
+        <v>-14.4981330054914</v>
       </c>
       <c r="C368" t="n">
-        <v>-18.1035207738078</v>
+        <v>-28.6493160099172</v>
       </c>
       <c r="D368" t="s">
         <v>6</v>
@@ -7753,10 +7753,10 @@
         <v>376</v>
       </c>
       <c r="B369" t="n">
-        <v>19.458560669197</v>
+        <v>-5.34990865761154</v>
       </c>
       <c r="C369" t="n">
-        <v>-18.0494472353404</v>
+        <v>12.9675922345912</v>
       </c>
       <c r="D369" t="s">
         <v>9</v>
@@ -7770,10 +7770,10 @@
         <v>377</v>
       </c>
       <c r="B370" t="n">
-        <v>3.58971859249968</v>
+        <v>51.4206811725513</v>
       </c>
       <c r="C370" t="n">
-        <v>10.1134546657272</v>
+        <v>8.4501663938087</v>
       </c>
       <c r="D370" t="s">
         <v>9</v>
@@ -7787,10 +7787,10 @@
         <v>378</v>
       </c>
       <c r="B371" t="n">
-        <v>-5.63057326627323</v>
+        <v>-51.3061549718381</v>
       </c>
       <c r="C371" t="n">
-        <v>4.88436360355457</v>
+        <v>7.79445378883165</v>
       </c>
       <c r="D371" t="s">
         <v>6</v>
@@ -7804,10 +7804,10 @@
         <v>379</v>
       </c>
       <c r="B372" t="n">
-        <v>7.98404839413206</v>
+        <v>-72.1365701059762</v>
       </c>
       <c r="C372" t="n">
-        <v>9.40463752293289</v>
+        <v>-0.00447196946264566</v>
       </c>
       <c r="D372" t="s">
         <v>6</v>
@@ -7821,10 +7821,10 @@
         <v>380</v>
       </c>
       <c r="B373" t="n">
-        <v>-6.56226325368817</v>
+        <v>-28.4667540591843</v>
       </c>
       <c r="C373" t="n">
-        <v>-3.1425199274611</v>
+        <v>-6.68872921611687</v>
       </c>
       <c r="D373" t="s">
         <v>6</v>
@@ -7838,10 +7838,10 @@
         <v>381</v>
       </c>
       <c r="B374" t="n">
-        <v>22.4021309934176</v>
+        <v>-2.30320709176913</v>
       </c>
       <c r="C374" t="n">
-        <v>16.1585679160723</v>
+        <v>-24.3252831859598</v>
       </c>
       <c r="D374" t="s">
         <v>6</v>
@@ -7855,10 +7855,10 @@
         <v>382</v>
       </c>
       <c r="B375" t="n">
-        <v>11.7468164378669</v>
+        <v>-76.9480171364894</v>
       </c>
       <c r="C375" t="n">
-        <v>-14.7099243239827</v>
+        <v>19.9092536018061</v>
       </c>
       <c r="D375" t="s">
         <v>6</v>

</xml_diff>